<commit_message>
minor correction: added "impossible" on algorithm column for "ART_SWEETENER_170201"
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S1_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S1_P2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63DF491-CA9D-45C1-AA2B-8ECD10161C4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8A4CB8-1EE5-4AE9-BD2D-63923C775C48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8B979143-186A-4DC0-ADB7-438B45FFD7D0}"/>
   </bookViews>
@@ -17,9 +17,9 @@
   </sheets>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="49152 - Personal View" guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
+    <customWorkbookView name="Siampani, Sofia Maria - Personal View" guid="{D25176B6-2194-4D8F-99D6-14D593512471}" mergeInterval="0" personalView="1" xWindow="960" windowWidth="960" windowHeight="977" activeSheetId="1"/>
     <customWorkbookView name="Osei, Tracy Bonsu - Personal View" guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
-    <customWorkbookView name="Siampani, Sofia Maria - Personal View" guid="{D25176B6-2194-4D8F-99D6-14D593512471}" mergeInterval="0" personalView="1" xWindow="960" windowWidth="960" windowHeight="977" activeSheetId="1"/>
-    <customWorkbookView name="49152 - Personal View" guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="333">
   <si>
     <t>index</t>
   </si>
@@ -1345,7 +1345,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1361,7 +1361,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1659,11 +1659,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5EEE99-8A14-4256-9AEF-BF43A09DA625}">
   <dimension ref="A1:K127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90:D92"/>
+    <sheetView tabSelected="1" topLeftCell="D91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I100" sqref="I100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
@@ -4976,8 +4976,12 @@
       <c r="G99" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="H99" s="29"/>
-      <c r="I99" s="29"/>
+      <c r="H99" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I99" s="29" t="s">
+        <v>31</v>
+      </c>
       <c r="J99" s="29" t="s">
         <v>31</v>
       </c>
@@ -5315,8 +5319,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" topLeftCell="A51">
-      <selection activeCell="G56" sqref="G56"/>
+    <customSheetView guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" topLeftCell="A2">
+      <selection activeCell="G12" sqref="G12"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -5325,8 +5329,8 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" topLeftCell="A2">
-      <selection activeCell="G12" sqref="G12"/>
+    <customSheetView guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" topLeftCell="A51">
+      <selection activeCell="G56" sqref="G56"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -5337,12 +5341,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5587,21 +5594,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9BE38D0-BD1C-4126-A2D1-5A24E80B0CB5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6BB7CB2-3E08-455A-88BD-99593455AB98}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5626,12 +5633,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6BB7CB2-3E08-455A-88BD-99593455AB98}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9BE38D0-BD1C-4126-A2D1-5A24E80B0CB5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
small adjustments to naming in dataschema, DPE's for P2. Removed one "_" in BMI_SDS_FUP
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S1_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S1_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C416FB11-198A-4370-BA4F-35ACA146801B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30EDB0F-0063-4EFF-A412-F147F604AA37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" xr2:uid="{8B979143-186A-4DC0-ADB7-438B45FFD7D0}"/>
   </bookViews>
@@ -17,9 +17,9 @@
   </sheets>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="49152 - Personal View" guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
+    <customWorkbookView name="Siampani, Sofia Maria - Personal View" guid="{D25176B6-2194-4D8F-99D6-14D593512471}" mergeInterval="0" personalView="1" xWindow="960" windowWidth="960" windowHeight="977" activeSheetId="1"/>
     <customWorkbookView name="Osei, Tracy Bonsu - Personal View" guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
-    <customWorkbookView name="Siampani, Sofia Maria - Personal View" guid="{D25176B6-2194-4D8F-99D6-14D593512471}" mergeInterval="0" personalView="1" xWindow="960" windowWidth="960" windowHeight="977" activeSheetId="1"/>
-    <customWorkbookView name="49152 - Personal View" guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -624,9 +624,6 @@
   </si>
   <si>
     <t>Body Mass index Standard Deviation Score at baseline (children studies)</t>
-  </si>
-  <si>
-    <t>BMI__SDS_FUP</t>
   </si>
   <si>
     <t>Body Mass index Standard Deviation Score at follow-up (children studies)</t>
@@ -1065,12 +1062,15 @@
   <si>
     <t xml:space="preserve">AV141 (sausage) + AV145 (ham) + AV147 (bacon) + AV150 (canned, frozen meat or meat products) + AV160 (other meat products) </t>
   </si>
+  <si>
+    <t>BMI_SDS_FUP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1659,11 +1659,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5EEE99-8A14-4256-9AEF-BF43A09DA625}">
   <dimension ref="A1:K127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I105" sqref="I105"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
@@ -1678,7 +1678,7 @@
     <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1713,30 +1713,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1">
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>321</v>
-      </c>
       <c r="H2" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>14</v>
@@ -1748,7 +1748,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="2" customFormat="1">
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="2" customFormat="1">
+    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>13</v>
@@ -1882,7 +1882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="2" customFormat="1">
+    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>10</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="2" customFormat="1">
+    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>11</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="2" customFormat="1">
+    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>15</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="2" customFormat="1">
+    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>16</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="2" customFormat="1">
+    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>18</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>20</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>22</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="2" customFormat="1">
+    <row r="24" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>23</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="13">
         <v>24</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="2" customFormat="1">
+    <row r="26" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13">
         <v>25</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>12</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>13</v>
@@ -2548,7 +2548,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="1" customFormat="1">
+    <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>26</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="2" customFormat="1">
+    <row r="28" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13">
         <v>27</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>12</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G28" s="13" t="s">
         <v>13</v>
@@ -2616,7 +2616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="2" customFormat="1">
+    <row r="29" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13">
         <v>28</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>12</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>13</v>
@@ -2651,7 +2651,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="2" customFormat="1">
+    <row r="30" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
         <v>29</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>12</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G30" s="13" t="s">
         <v>13</v>
@@ -2686,7 +2686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="2" customFormat="1">
+    <row r="31" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13">
         <v>30</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="2" customFormat="1">
+    <row r="32" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="2" customFormat="1">
+    <row r="33" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>32</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="2" customFormat="1">
+    <row r="34" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="2" customFormat="1">
+    <row r="35" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
         <v>34</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="2" customFormat="1">
+    <row r="36" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="2" customFormat="1">
+    <row r="37" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>36</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="2" customFormat="1">
+    <row r="38" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9">
         <v>37</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="39" spans="1:11" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>38</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="2" customFormat="1">
+    <row r="40" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9">
         <v>39</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="2" customFormat="1">
+    <row r="41" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13">
         <v>40</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="9">
         <v>41</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <v>42</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="2" customFormat="1">
+    <row r="44" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13">
         <v>43</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="13">
         <v>44</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="1" customFormat="1">
+    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>46</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="2" customFormat="1">
+    <row r="48" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="13">
         <v>47</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>12</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G48" s="13" t="s">
         <v>13</v>
@@ -3290,7 +3290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="2" customFormat="1">
+    <row r="49" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
         <v>48</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="2" customFormat="1">
+    <row r="50" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>49</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>12</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G50" s="13" t="s">
         <v>13</v>
@@ -3360,7 +3360,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="2" customFormat="1">
+    <row r="51" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13">
         <v>50</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="9">
         <v>51</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="13">
         <v>52</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="2" customFormat="1">
+    <row r="54" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9">
         <v>53</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="13">
         <v>54</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="13">
         <v>56</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="9">
         <v>57</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="13">
         <v>58</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="13">
         <v>60</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="9">
         <v>61</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="13">
         <v>62</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="9">
         <v>63</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="19">
         <v>64</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="19">
         <v>65</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="19">
         <v>66</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="19">
         <v>67</v>
       </c>
@@ -3958,15 +3958,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="19">
         <v>68</v>
       </c>
       <c r="B69" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="C69" s="17" t="s">
         <v>198</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>199</v>
       </c>
       <c r="D69" s="19" t="s">
         <v>35</v>
@@ -3991,15 +3991,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="19">
         <v>69</v>
       </c>
       <c r="B70" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="C70" s="13" t="s">
         <v>200</v>
-      </c>
-      <c r="C70" s="13" t="s">
-        <v>201</v>
       </c>
       <c r="D70" s="19" t="s">
         <v>35</v>
@@ -4024,15 +4024,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="19">
         <v>70</v>
       </c>
       <c r="B71" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="C71" s="13" t="s">
         <v>202</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>203</v>
       </c>
       <c r="D71" s="19" t="s">
         <v>35</v>
@@ -4057,15 +4057,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="19">
         <v>71</v>
       </c>
       <c r="B72" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="C72" s="13" t="s">
         <v>204</v>
-      </c>
-      <c r="C72" s="13" t="s">
-        <v>205</v>
       </c>
       <c r="D72" s="19" t="s">
         <v>35</v>
@@ -4090,15 +4090,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="19">
         <v>72</v>
       </c>
       <c r="B73" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="C73" s="13" t="s">
         <v>206</v>
-      </c>
-      <c r="C73" s="13" t="s">
-        <v>207</v>
       </c>
       <c r="D73" s="19" t="s">
         <v>35</v>
@@ -4123,15 +4123,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="19">
         <v>73</v>
       </c>
       <c r="B74" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="C74" s="13" t="s">
         <v>208</v>
-      </c>
-      <c r="C74" s="13" t="s">
-        <v>209</v>
       </c>
       <c r="D74" s="19" t="s">
         <v>35</v>
@@ -4156,15 +4156,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="2" customFormat="1">
+    <row r="75" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="21">
         <v>74</v>
       </c>
       <c r="B75" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="C75" s="45" t="s">
         <v>210</v>
-      </c>
-      <c r="C75" s="45" t="s">
-        <v>211</v>
       </c>
       <c r="D75" s="19" t="s">
         <v>35</v>
@@ -4189,15 +4189,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:11" s="2" customFormat="1">
+    <row r="76" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="43">
         <v>75</v>
       </c>
       <c r="B76" s="41" t="s">
+        <v>211</v>
+      </c>
+      <c r="C76" s="42" t="s">
         <v>212</v>
-      </c>
-      <c r="C76" s="42" t="s">
-        <v>213</v>
       </c>
       <c r="D76" s="19" t="s">
         <v>35</v>
@@ -4222,24 +4222,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="19">
         <v>76</v>
       </c>
       <c r="B77" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="C77" s="47" t="s">
         <v>214</v>
       </c>
-      <c r="C77" s="47" t="s">
+      <c r="D77" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E77" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F77" s="26" t="s">
         <v>215</v>
-      </c>
-      <c r="D77" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E77" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F77" s="26" t="s">
-        <v>216</v>
       </c>
       <c r="G77" s="19" t="s">
         <v>13</v>
@@ -4255,24 +4255,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="19">
         <v>77</v>
       </c>
       <c r="B78" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="C78" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="C78" s="13" t="s">
+      <c r="D78" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78" s="26" t="s">
         <v>218</v>
-      </c>
-      <c r="D78" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F78" s="26" t="s">
-        <v>219</v>
       </c>
       <c r="G78" s="19" t="s">
         <v>13</v>
@@ -4288,24 +4288,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="19">
         <v>78</v>
       </c>
       <c r="B79" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C79" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="C79" s="13" t="s">
+      <c r="D79" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E79" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79" s="26" t="s">
         <v>221</v>
-      </c>
-      <c r="D79" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E79" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F79" s="26" t="s">
-        <v>222</v>
       </c>
       <c r="G79" s="19" t="s">
         <v>13</v>
@@ -4321,24 +4321,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="19">
         <v>79</v>
       </c>
       <c r="B80" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C80" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="C80" s="13" t="s">
+      <c r="D80" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" s="26" t="s">
         <v>224</v>
-      </c>
-      <c r="D80" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E80" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F80" s="26" t="s">
-        <v>225</v>
       </c>
       <c r="G80" s="19" t="s">
         <v>13</v>
@@ -4354,24 +4354,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="19">
         <v>80</v>
       </c>
       <c r="B81" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="C81" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="C81" s="13" t="s">
+      <c r="D81" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E81" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81" s="26" t="s">
         <v>227</v>
-      </c>
-      <c r="D81" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E81" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F81" s="26" t="s">
-        <v>228</v>
       </c>
       <c r="G81" s="19" t="s">
         <v>13</v>
@@ -4387,24 +4387,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="21">
         <v>81</v>
       </c>
       <c r="B82" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C82" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="C82" s="13" t="s">
+      <c r="D82" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F82" s="26" t="s">
         <v>230</v>
-      </c>
-      <c r="D82" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F82" s="26" t="s">
-        <v>231</v>
       </c>
       <c r="G82" s="19" t="s">
         <v>13</v>
@@ -4420,24 +4420,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="19">
         <v>82</v>
       </c>
       <c r="B83" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="C83" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="C83" s="13" t="s">
+      <c r="D83" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E83" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F83" s="26" t="s">
         <v>233</v>
-      </c>
-      <c r="D83" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F83" s="26" t="s">
-        <v>234</v>
       </c>
       <c r="G83" s="19" t="s">
         <v>13</v>
@@ -4453,24 +4453,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="19">
         <v>83</v>
       </c>
       <c r="B84" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="C84" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="C84" s="13" t="s">
+      <c r="D84" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F84" s="26" t="s">
         <v>236</v>
-      </c>
-      <c r="D84" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F84" s="26" t="s">
-        <v>237</v>
       </c>
       <c r="G84" s="19" t="s">
         <v>13</v>
@@ -4486,24 +4486,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="19">
         <v>84</v>
       </c>
       <c r="B85" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C85" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="C85" s="13" t="s">
+      <c r="D85" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E85" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F85" s="26" t="s">
         <v>239</v>
-      </c>
-      <c r="D85" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E85" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F85" s="26" t="s">
-        <v>240</v>
       </c>
       <c r="G85" s="19" t="s">
         <v>13</v>
@@ -4519,24 +4519,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="19">
         <v>85</v>
       </c>
       <c r="B86" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="C86" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="C86" s="13" t="s">
+      <c r="D86" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E86" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86" s="26" t="s">
         <v>242</v>
-      </c>
-      <c r="D86" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E86" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F86" s="26" t="s">
-        <v>243</v>
       </c>
       <c r="G86" s="19" t="s">
         <v>13</v>
@@ -4552,15 +4552,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="19">
         <v>86</v>
       </c>
       <c r="B87" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="C87" s="13" t="s">
         <v>244</v>
-      </c>
-      <c r="C87" s="13" t="s">
-        <v>245</v>
       </c>
       <c r="D87" s="19" t="s">
         <v>35</v>
@@ -4585,15 +4585,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="19">
         <v>87</v>
       </c>
       <c r="B88" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="C88" s="13" t="s">
         <v>246</v>
-      </c>
-      <c r="C88" s="13" t="s">
-        <v>247</v>
       </c>
       <c r="D88" s="19" t="s">
         <v>35</v>
@@ -4618,24 +4618,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="21">
         <v>88</v>
       </c>
       <c r="B89" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="C89" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="C89" s="13" t="s">
+      <c r="D89" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E89" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F89" s="28" t="s">
         <v>249</v>
-      </c>
-      <c r="D89" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E89" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F89" s="28" t="s">
-        <v>250</v>
       </c>
       <c r="G89" s="19" t="s">
         <v>13</v>
@@ -4651,24 +4651,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="19">
         <v>89</v>
       </c>
       <c r="B90" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="C90" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="C90" s="13" t="s">
+      <c r="D90" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E90" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F90" s="19" t="s">
         <v>252</v>
-      </c>
-      <c r="D90" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E90" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F90" s="19" t="s">
-        <v>253</v>
       </c>
       <c r="G90" s="19" t="s">
         <v>13</v>
@@ -4684,15 +4684,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="19">
         <v>90</v>
       </c>
       <c r="B91" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="C91" s="13" t="s">
         <v>254</v>
-      </c>
-      <c r="C91" s="13" t="s">
-        <v>255</v>
       </c>
       <c r="D91" s="19" t="s">
         <v>35</v>
@@ -4717,15 +4717,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="19">
         <v>91</v>
       </c>
       <c r="B92" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="C92" s="13" t="s">
         <v>256</v>
-      </c>
-      <c r="C92" s="13" t="s">
-        <v>257</v>
       </c>
       <c r="D92" s="19" t="s">
         <v>35</v>
@@ -4750,24 +4750,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="19">
         <v>92</v>
       </c>
       <c r="B93" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="C93" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C93" s="13" t="s">
+      <c r="D93" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F93" s="19" t="s">
         <v>259</v>
-      </c>
-      <c r="D93" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E93" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F93" s="19" t="s">
-        <v>260</v>
       </c>
       <c r="G93" s="19" t="s">
         <v>13</v>
@@ -4783,30 +4783,30 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="19">
         <v>93</v>
       </c>
       <c r="B94" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="C94" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="C94" s="13" t="s">
+      <c r="D94" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E94" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F94" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="D94" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E94" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F94" s="19" t="s">
+      <c r="G94" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="G94" s="19" t="s">
+      <c r="H94" s="19" t="s">
         <v>264</v>
-      </c>
-      <c r="H94" s="19" t="s">
-        <v>265</v>
       </c>
       <c r="I94" s="19"/>
       <c r="J94" s="19" t="s">
@@ -4816,155 +4816,155 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:11" s="4" customFormat="1" ht="57.6">
+    <row r="95" spans="1:11" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A95" s="19">
         <v>94</v>
       </c>
       <c r="B95" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="C95" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="C95" s="30" t="s">
+      <c r="D95" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E95" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="D95" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E95" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F95" s="31" t="s">
+      <c r="G95" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="H95" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="G95" s="48" t="s">
-        <v>264</v>
-      </c>
-      <c r="H95" s="32" t="s">
+      <c r="I95" s="33" t="s">
         <v>269</v>
       </c>
-      <c r="I95" s="33" t="s">
+      <c r="J95" s="29" t="s">
         <v>270</v>
       </c>
-      <c r="J95" s="29" t="s">
+      <c r="K95" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="K95" s="29" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" s="4" customFormat="1" ht="28.8">
+    </row>
+    <row r="96" spans="1:11" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="21">
         <v>95</v>
       </c>
       <c r="B96" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="C96" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="C96" s="34" t="s">
+      <c r="D96" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E96" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F96" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="D96" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E96" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F96" s="29" t="s">
+      <c r="G96" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="H96" s="29" t="s">
         <v>275</v>
       </c>
-      <c r="G96" s="48" t="s">
-        <v>264</v>
-      </c>
-      <c r="H96" s="29" t="s">
+      <c r="I96" s="33" t="s">
         <v>276</v>
       </c>
-      <c r="I96" s="33" t="s">
-        <v>277</v>
-      </c>
       <c r="J96" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="K96" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="K96" s="29" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" s="4" customFormat="1">
+    </row>
+    <row r="97" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="19">
         <v>96</v>
       </c>
       <c r="B97" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="C97" s="34" t="s">
         <v>278</v>
       </c>
-      <c r="C97" s="34" t="s">
+      <c r="D97" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E97" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97" s="35" t="s">
         <v>279</v>
       </c>
-      <c r="D97" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E97" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F97" s="35" t="s">
+      <c r="G97" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H97" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="I97" s="35" t="s">
         <v>280</v>
       </c>
-      <c r="G97" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="H97" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I97" s="35" t="s">
-        <v>281</v>
-      </c>
       <c r="J97" s="29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K97" s="29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:11" s="4" customFormat="1" ht="28.8">
+    <row r="98" spans="1:11" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="19">
         <v>97</v>
       </c>
       <c r="B98" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="C98" s="34" t="s">
         <v>282</v>
       </c>
-      <c r="C98" s="34" t="s">
+      <c r="D98" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E98" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F98" s="29" t="s">
         <v>283</v>
       </c>
-      <c r="D98" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E98" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F98" s="29" t="s">
+      <c r="G98" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="H98" s="29" t="s">
         <v>284</v>
       </c>
-      <c r="G98" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="H98" s="29" t="s">
+      <c r="I98" s="33" t="s">
         <v>285</v>
       </c>
-      <c r="I98" s="33" t="s">
-        <v>286</v>
-      </c>
       <c r="J98" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="K98" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="K98" s="29" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" s="4" customFormat="1">
+    </row>
+    <row r="99" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="19">
         <v>98</v>
       </c>
       <c r="B99" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="C99" s="34" t="s">
         <v>287</v>
-      </c>
-      <c r="C99" s="34" t="s">
-        <v>288</v>
       </c>
       <c r="D99" s="29" t="s">
         <v>35</v>
@@ -4989,156 +4989,156 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:11" s="4" customFormat="1" ht="115.2">
+    <row r="100" spans="1:11" s="4" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A100" s="19">
         <v>99</v>
       </c>
       <c r="B100" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="C100" s="34" t="s">
         <v>289</v>
       </c>
-      <c r="C100" s="34" t="s">
+      <c r="D100" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E100" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F100" s="33" t="s">
         <v>290</v>
       </c>
-      <c r="D100" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E100" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F100" s="33" t="s">
+      <c r="G100" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="H100" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="G100" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="H100" s="33" t="s">
+      <c r="I100" s="33" t="s">
         <v>292</v>
       </c>
-      <c r="I100" s="33" t="s">
-        <v>293</v>
-      </c>
       <c r="J100" s="29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K100" s="29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="101" spans="1:11" s="4" customFormat="1">
+    <row r="101" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="19">
         <v>100</v>
       </c>
       <c r="B101" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="C101" s="20" t="s">
         <v>294</v>
       </c>
-      <c r="C101" s="20" t="s">
+      <c r="D101" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E101" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F101" s="37" t="s">
         <v>295</v>
       </c>
-      <c r="D101" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E101" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F101" s="37" t="s">
+      <c r="G101" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H101" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="I101" s="37" t="s">
         <v>296</v>
       </c>
-      <c r="G101" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="H101" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="I101" s="37" t="s">
-        <v>297</v>
-      </c>
       <c r="J101" s="29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K101" s="29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:11" s="4" customFormat="1" ht="273.60000000000002">
+    <row r="102" spans="1:11" s="4" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A102" s="19">
         <v>101</v>
       </c>
       <c r="B102" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="C102" s="30" t="s">
         <v>298</v>
       </c>
-      <c r="C102" s="30" t="s">
+      <c r="D102" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E102" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F102" s="31" t="s">
         <v>299</v>
       </c>
-      <c r="D102" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E102" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F102" s="31" t="s">
+      <c r="G102" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="H102" s="31" t="s">
         <v>300</v>
       </c>
-      <c r="G102" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="H102" s="31" t="s">
+      <c r="I102" s="33" t="s">
         <v>301</v>
       </c>
-      <c r="I102" s="33" t="s">
-        <v>302</v>
-      </c>
       <c r="J102" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="K102" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="K102" s="29" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" s="4" customFormat="1" ht="43.2">
+    </row>
+    <row r="103" spans="1:11" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A103" s="21">
         <v>102</v>
       </c>
       <c r="B103" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="C103" s="34" t="s">
         <v>303</v>
       </c>
-      <c r="C103" s="34" t="s">
+      <c r="D103" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E103" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F103" s="33" t="s">
         <v>304</v>
       </c>
-      <c r="D103" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E103" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F103" s="33" t="s">
+      <c r="G103" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="H103" s="33" t="s">
         <v>305</v>
       </c>
-      <c r="G103" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="H103" s="33" t="s">
+      <c r="I103" s="38" t="s">
         <v>306</v>
       </c>
-      <c r="I103" s="38" t="s">
-        <v>307</v>
-      </c>
       <c r="J103" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="K103" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="K103" s="29" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" s="4" customFormat="1" ht="43.2">
+    </row>
+    <row r="104" spans="1:11" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A104" s="19">
         <v>103</v>
       </c>
       <c r="B104" s="29" t="s">
+        <v>307</v>
+      </c>
+      <c r="C104" s="34" t="s">
         <v>308</v>
       </c>
-      <c r="C104" s="34" t="s">
-        <v>309</v>
-      </c>
       <c r="D104" s="29" t="s">
         <v>35</v>
       </c>
@@ -5146,181 +5146,181 @@
         <v>12</v>
       </c>
       <c r="F104" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="G104" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="H104" s="33" t="s">
         <v>330</v>
       </c>
-      <c r="G104" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="H104" s="33" t="s">
+      <c r="I104" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="I104" s="33" t="s">
-        <v>332</v>
-      </c>
       <c r="J104" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="K104" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="K104" s="29" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" s="4" customFormat="1">
+    </row>
+    <row r="105" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="19">
         <v>104</v>
       </c>
       <c r="B105" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="C105" s="34" t="s">
         <v>310</v>
       </c>
-      <c r="C105" s="34" t="s">
+      <c r="D105" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E105" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F105" s="29" t="s">
         <v>311</v>
       </c>
-      <c r="D105" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E105" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F105" s="29" t="s">
+      <c r="G105" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="H105" s="29" t="s">
         <v>312</v>
       </c>
-      <c r="G105" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="H105" s="29" t="s">
+      <c r="I105" s="38" t="s">
         <v>313</v>
       </c>
-      <c r="I105" s="38" t="s">
-        <v>314</v>
-      </c>
       <c r="J105" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="K105" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="K105" s="29" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" s="4" customFormat="1">
+    </row>
+    <row r="106" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="19">
         <v>105</v>
       </c>
       <c r="B106" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="C106" s="34" t="s">
         <v>315</v>
       </c>
-      <c r="C106" s="34" t="s">
+      <c r="D106" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E106" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F106" s="35" t="s">
         <v>316</v>
       </c>
-      <c r="D106" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E106" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F106" s="35" t="s">
+      <c r="G106" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H106" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I106" s="35" t="s">
         <v>317</v>
       </c>
-      <c r="G106" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="H106" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="I106" s="35" t="s">
-        <v>318</v>
-      </c>
       <c r="J106" s="29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K106" s="29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:11" s="4" customFormat="1">
+    <row r="107" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C107" s="5"/>
       <c r="E107" s="3"/>
       <c r="I107" s="3"/>
     </row>
-    <row r="108" spans="1:11" s="4" customFormat="1">
+    <row r="108" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E108" s="3"/>
       <c r="I108" s="3"/>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E109" s="1"/>
       <c r="I109" s="1"/>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E110" s="1"/>
       <c r="I110" s="1"/>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E111" s="1"/>
       <c r="I111" s="1"/>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E112" s="1"/>
       <c r="I112" s="1"/>
     </row>
-    <row r="113" spans="5:9">
+    <row r="113" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E113" s="1"/>
       <c r="I113" s="1"/>
     </row>
-    <row r="114" spans="5:9">
+    <row r="114" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E114" s="1"/>
       <c r="I114" s="1"/>
     </row>
-    <row r="115" spans="5:9">
+    <row r="115" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E115" s="1"/>
       <c r="I115" s="1"/>
     </row>
-    <row r="116" spans="5:9">
+    <row r="116" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E116" s="1"/>
       <c r="I116" s="1"/>
     </row>
-    <row r="117" spans="5:9">
+    <row r="117" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E117" s="1"/>
       <c r="I117" s="1"/>
     </row>
-    <row r="118" spans="5:9">
+    <row r="118" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E118" s="1"/>
       <c r="I118" s="1"/>
     </row>
-    <row r="119" spans="5:9">
+    <row r="119" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E119" s="1"/>
       <c r="I119" s="1"/>
     </row>
-    <row r="120" spans="5:9">
+    <row r="120" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E120" s="1"/>
       <c r="I120" s="1"/>
     </row>
-    <row r="121" spans="5:9">
+    <row r="121" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E121" s="1"/>
       <c r="I121" s="1"/>
     </row>
-    <row r="122" spans="5:9">
+    <row r="122" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E122" s="1"/>
       <c r="I122" s="1"/>
     </row>
-    <row r="123" spans="5:9">
+    <row r="123" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E123" s="1"/>
       <c r="I123" s="1"/>
     </row>
-    <row r="124" spans="5:9">
+    <row r="124" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E124" s="1"/>
       <c r="I124" s="1"/>
     </row>
-    <row r="125" spans="5:9">
+    <row r="125" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E125" s="1"/>
       <c r="I125" s="1"/>
     </row>
-    <row r="126" spans="5:9">
+    <row r="126" spans="5:9" x14ac:dyDescent="0.3">
       <c r="I126" s="1"/>
     </row>
-    <row r="127" spans="5:9">
+    <row r="127" spans="5:9" x14ac:dyDescent="0.3">
       <c r="I127" s="1"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" topLeftCell="A51">
-      <selection activeCell="G56" sqref="G56"/>
+    <customSheetView guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" topLeftCell="A2">
+      <selection activeCell="G12" sqref="G12"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -5329,8 +5329,8 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" topLeftCell="A2">
-      <selection activeCell="G12" sqref="G12"/>
+    <customSheetView guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" topLeftCell="A51">
+      <selection activeCell="G56" sqref="G56"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -5341,15 +5341,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5590,6 +5581,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -5603,14 +5603,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9BE38D0-BD1C-4126-A2D1-5A24E80B0CB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01209340-F0B9-4FEB-870E-F887EE00E421}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5629,6 +5621,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9BE38D0-BD1C-4126-A2D1-5A24E80B0CB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6BB7CB2-3E08-455A-88BD-99593455AB98}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
final description label edit for P2 of Dataschema and DPE's
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S1_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S1_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27A55F3-3A1D-4660-96ED-E1B9BE3A2BA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4130545-D28E-4A74-8653-1BB17205105B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" xr2:uid="{8B979143-186A-4DC0-ADB7-438B45FFD7D0}"/>
   </bookViews>
@@ -17,9 +17,9 @@
   </sheets>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Osei, Tracy Bonsu - Personal View" guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
+    <customWorkbookView name="Siampani, Sofia Maria - Personal View" guid="{D25176B6-2194-4D8F-99D6-14D593512471}" mergeInterval="0" personalView="1" xWindow="960" windowWidth="960" windowHeight="977" activeSheetId="1"/>
     <customWorkbookView name="49152 - Personal View" guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
-    <customWorkbookView name="Siampani, Sofia Maria - Personal View" guid="{D25176B6-2194-4D8F-99D6-14D593512471}" mergeInterval="0" personalView="1" xWindow="960" windowWidth="960" windowHeight="977" activeSheetId="1"/>
-    <customWorkbookView name="Osei, Tracy Bonsu - Personal View" guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -233,9 +233,6 @@
     <t>CONTRACEPTIVE</t>
   </si>
   <si>
-    <t xml:space="preserve">Use of contraceptive pills or injections </t>
-  </si>
-  <si>
     <t>LIVE_BIRTHS</t>
   </si>
   <si>
@@ -281,9 +278,6 @@
     <t>PREV_DIAB</t>
   </si>
   <si>
-    <t>History of diabetes (T2DM)</t>
-  </si>
-  <si>
     <t>prev_dm_16</t>
   </si>
   <si>
@@ -380,21 +374,12 @@
     <t>MELANOMA_SCREEN</t>
   </si>
   <si>
-    <t>Screening, Skin cancer</t>
-  </si>
-  <si>
     <t>MAMMO_SCREEN</t>
   </si>
   <si>
-    <t>Screening, Mammography</t>
-  </si>
-  <si>
     <t>CERVICAL_SCREEN</t>
   </si>
   <si>
-    <t>Cervical screening, smear test</t>
-  </si>
-  <si>
     <t>MED_STAT</t>
   </si>
   <si>
@@ -575,9 +560,6 @@
     <t>TYPE_CANCER</t>
   </si>
   <si>
-    <t>Type of cancer</t>
-  </si>
-  <si>
     <t>AGE_CANCER</t>
   </si>
   <si>
@@ -629,18 +611,12 @@
     <t>BMI</t>
   </si>
   <si>
-    <t>Body Mass index at baseline</t>
-  </si>
-  <si>
     <t>atbmi</t>
   </si>
   <si>
     <t>BMI_FUP</t>
   </si>
   <si>
-    <t>Body Mass index at follow-up</t>
-  </si>
-  <si>
     <t>k4tbmi</t>
   </si>
   <si>
@@ -656,15 +632,9 @@
     <t>BMI_SDS</t>
   </si>
   <si>
-    <t>Body Mass index Standard Deviation Score at baseline (children studies)</t>
-  </si>
-  <si>
     <t>BMI_SDS_FUP</t>
   </si>
   <si>
-    <t>Body Mass index Standard Deviation Score at follow-up (children studies)</t>
-  </si>
-  <si>
     <t>WAIST_FUP</t>
   </si>
   <si>
@@ -704,15 +674,9 @@
     <t>BODY_FAT_FUP</t>
   </si>
   <si>
-    <t>Body fat at follow-up</t>
-  </si>
-  <si>
     <t>BODY_FAT</t>
   </si>
   <si>
-    <t>Body fat at baseline</t>
-  </si>
-  <si>
     <t>AGE_ANTH_FUP</t>
   </si>
   <si>
@@ -848,9 +812,6 @@
     <t>GL</t>
   </si>
   <si>
-    <t xml:space="preserve">Daily glycaemic load </t>
-  </si>
-  <si>
     <t>SODIUM</t>
   </si>
   <si>
@@ -899,9 +860,6 @@
     <t>CAKES_12</t>
   </si>
   <si>
-    <t>Intake of cakes and fine bakery wares [g/d]</t>
-  </si>
-  <si>
     <t>AV540; AV570</t>
   </si>
   <si>
@@ -914,9 +872,6 @@
     <t>FRUITVEG_JUICE_1301</t>
   </si>
   <si>
-    <t>Intake of fruit and vegetable juices and nectars [g/d]</t>
-  </si>
-  <si>
     <t>AV810</t>
   </si>
   <si>
@@ -924,9 +879,6 @@
   </si>
   <si>
     <t>SOFTDRINKS_1302</t>
-  </si>
-  <si>
-    <t>Intake of soft drinks (flavoured, no fruit) [g/d]</t>
   </si>
   <si>
     <t>AV825; AV829</t>
@@ -971,9 +923,6 @@
     <t>LEGUMES_TOT_03</t>
   </si>
   <si>
-    <t>Legumes intake [g/d]</t>
-  </si>
-  <si>
     <t xml:space="preserve">AV491 </t>
   </si>
   <si>
@@ -981,9 +930,6 @@
   </si>
   <si>
     <t>FRUITS_TOT_04</t>
-  </si>
-  <si>
-    <t>intake of any type of RPCs of fruit nature [g/d]</t>
   </si>
   <si>
     <t>AV310; AV311; AV315;AV321; AV323;
@@ -1091,6 +1037,60 @@
   </si>
   <si>
     <t>5 (7_d_FR_w)</t>
+  </si>
+  <si>
+    <t>Use of contraceptive pills or injections</t>
+  </si>
+  <si>
+    <t>History of diabetes</t>
+  </si>
+  <si>
+    <t>Screening, skin cancer</t>
+  </si>
+  <si>
+    <t>Screening, mammography</t>
+  </si>
+  <si>
+    <t>Screening cervical, smear test</t>
+  </si>
+  <si>
+    <t>Type of Cancer (ICD 10, 3 digits,e.g. C18)</t>
+  </si>
+  <si>
+    <t>Body Mass Index at baseline</t>
+  </si>
+  <si>
+    <t>Body Mass Index at follow-up</t>
+  </si>
+  <si>
+    <t>Body Mass Index Standard Deviation Score at baseline (children studies)</t>
+  </si>
+  <si>
+    <t>Body Mass Index Standard Deviation Score at follow-up (children studies)</t>
+  </si>
+  <si>
+    <t>Body fat precent at follow-up</t>
+  </si>
+  <si>
+    <t>Body fat precent at baseline</t>
+  </si>
+  <si>
+    <t>Daily glycaemic load</t>
+  </si>
+  <si>
+    <t>Intake of cakes and fine bakery products [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of fruit and vegetable juices [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of soft drinks [g/d]</t>
+  </si>
+  <si>
+    <t>Total legumes intake [g/d]</t>
+  </si>
+  <si>
+    <t>Total fruit intake [g/d]</t>
   </si>
 </sst>
 </file>
@@ -1684,7 +1684,7 @@
   <dimension ref="A1:K129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E110" sqref="E110"/>
+      <selection activeCell="C2" sqref="C2:C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2248,7 +2248,7 @@
         <v>66</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>67</v>
+        <v>324</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>21</v>
@@ -2278,10 +2278,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>68</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>69</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>21</v>
@@ -2311,10 +2311,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>26</v>
@@ -2344,10 +2344,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>26</v>
@@ -2377,19 +2377,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="D21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="18" t="s">
         <v>75</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>76</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>23</v>
@@ -2410,10 +2410,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>77</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>78</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>26</v>
@@ -2443,19 +2443,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="D23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="18" t="s">
         <v>80</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>81</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>23</v>
@@ -2476,10 +2476,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>83</v>
+        <v>325</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>21</v>
@@ -2488,7 +2488,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>23</v>
@@ -2509,10 +2509,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>21</v>
@@ -2521,7 +2521,7 @@
         <v>14</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>23</v>
@@ -2542,10 +2542,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>21</v>
@@ -2554,7 +2554,7 @@
         <v>14</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>23</v>
@@ -2563,7 +2563,7 @@
         <v>23</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J26" s="12" t="s">
         <v>17</v>
@@ -2577,10 +2577,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>21</v>
@@ -2610,10 +2610,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>21</v>
@@ -2622,7 +2622,7 @@
         <v>14</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>23</v>
@@ -2631,7 +2631,7 @@
         <v>23</v>
       </c>
       <c r="I28" s="38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J28" s="12" t="s">
         <v>58</v>
@@ -2645,10 +2645,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>21</v>
@@ -2657,7 +2657,7 @@
         <v>14</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>23</v>
@@ -2666,7 +2666,7 @@
         <v>23</v>
       </c>
       <c r="I29" s="39" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J29" s="12" t="s">
         <v>58</v>
@@ -2680,10 +2680,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>21</v>
@@ -2692,7 +2692,7 @@
         <v>14</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>23</v>
@@ -2701,7 +2701,7 @@
         <v>23</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>58</v>
@@ -2715,10 +2715,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>21</v>
@@ -2728,7 +2728,7 @@
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>37</v>
@@ -2748,10 +2748,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>21</v>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>37</v>
@@ -2781,10 +2781,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>21</v>
@@ -2794,7 +2794,7 @@
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>37</v>
@@ -2803,7 +2803,7 @@
         <v>38</v>
       </c>
       <c r="J33" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K33" s="12" t="s">
         <v>38</v>
@@ -2814,10 +2814,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>21</v>
@@ -2827,7 +2827,7 @@
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>37</v>
@@ -2847,10 +2847,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>116</v>
+        <v>326</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>21</v>
@@ -2860,7 +2860,7 @@
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H35" s="12" t="s">
         <v>37</v>
@@ -2880,10 +2880,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>118</v>
+        <v>327</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>21</v>
@@ -2893,7 +2893,7 @@
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H36" s="12" t="s">
         <v>37</v>
@@ -2913,10 +2913,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>120</v>
+        <v>328</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>21</v>
@@ -2926,7 +2926,7 @@
       </c>
       <c r="F37" s="12"/>
       <c r="G37" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H37" s="12" t="s">
         <v>37</v>
@@ -2946,10 +2946,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>21</v>
@@ -2958,7 +2958,7 @@
         <v>14</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>23</v>
@@ -2979,10 +2979,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>21</v>
@@ -2992,7 +2992,7 @@
       </c>
       <c r="F39" s="12"/>
       <c r="G39" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H39" s="12" t="s">
         <v>37</v>
@@ -3012,10 +3012,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>21</v>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H40" s="12" t="s">
         <v>37</v>
@@ -3045,10 +3045,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>26</v>
@@ -3058,7 +3058,7 @@
       </c>
       <c r="F41" s="12"/>
       <c r="G41" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H41" s="12" t="s">
         <v>37</v>
@@ -3078,10 +3078,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>21</v>
@@ -3091,7 +3091,7 @@
       </c>
       <c r="F42" s="12"/>
       <c r="G42" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H42" s="12" t="s">
         <v>37</v>
@@ -3111,10 +3111,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>26</v>
@@ -3124,7 +3124,7 @@
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H43" s="7" t="s">
         <v>37</v>
@@ -3144,10 +3144,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D44" s="12" t="s">
         <v>21</v>
@@ -3156,7 +3156,7 @@
         <v>14</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G44" s="12" t="s">
         <v>23</v>
@@ -3165,7 +3165,7 @@
         <v>23</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J44" s="12" t="s">
         <v>17</v>
@@ -3179,10 +3179,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>26</v>
@@ -3191,7 +3191,7 @@
         <v>14</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>23</v>
@@ -3200,7 +3200,7 @@
         <v>23</v>
       </c>
       <c r="I45" s="21" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="J45" s="12" t="s">
         <v>17</v>
@@ -3214,10 +3214,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>21</v>
@@ -3226,7 +3226,7 @@
         <v>14</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G46" s="7" t="s">
         <v>23</v>
@@ -3235,7 +3235,7 @@
         <v>23</v>
       </c>
       <c r="I46" s="24" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="J46" s="12" t="s">
         <v>17</v>
@@ -3249,10 +3249,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>26</v>
@@ -3261,7 +3261,7 @@
         <v>14</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>23</v>
@@ -3270,7 +3270,7 @@
         <v>23</v>
       </c>
       <c r="I47" s="21" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="J47" s="7" t="s">
         <v>17</v>
@@ -3284,10 +3284,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>21</v>
@@ -3296,7 +3296,7 @@
         <v>14</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G48" s="12" t="s">
         <v>23</v>
@@ -3305,7 +3305,7 @@
         <v>23</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J48" s="19" t="s">
         <v>17</v>
@@ -3319,10 +3319,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>26</v>
@@ -3331,7 +3331,7 @@
         <v>14</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>23</v>
@@ -3340,7 +3340,7 @@
         <v>23</v>
       </c>
       <c r="I49" s="13" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J49" s="12" t="s">
         <v>17</v>
@@ -3354,10 +3354,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>21</v>
@@ -3366,7 +3366,7 @@
         <v>14</v>
       </c>
       <c r="F50" s="19" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G50" s="12" t="s">
         <v>23</v>
@@ -3375,7 +3375,7 @@
         <v>23</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="J50" s="12" t="s">
         <v>17</v>
@@ -3389,10 +3389,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>26</v>
@@ -3401,7 +3401,7 @@
         <v>14</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>23</v>
@@ -3410,7 +3410,7 @@
         <v>23</v>
       </c>
       <c r="I51" s="21" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="J51" s="12" t="s">
         <v>17</v>
@@ -3424,10 +3424,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>21</v>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="F52" s="12"/>
       <c r="G52" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H52" s="12" t="s">
         <v>37</v>
@@ -3457,10 +3457,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>26</v>
@@ -3470,7 +3470,7 @@
       </c>
       <c r="F53" s="12"/>
       <c r="G53" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H53" s="12" t="s">
         <v>37</v>
@@ -3490,10 +3490,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>21</v>
@@ -3503,7 +3503,7 @@
       </c>
       <c r="F54" s="12"/>
       <c r="G54" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H54" s="12" t="s">
         <v>37</v>
@@ -3523,10 +3523,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>26</v>
@@ -3536,7 +3536,7 @@
       </c>
       <c r="F55" s="12"/>
       <c r="G55" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H55" s="12" t="s">
         <v>37</v>
@@ -3556,10 +3556,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>21</v>
@@ -3568,7 +3568,7 @@
         <v>14</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="G56" s="7" t="s">
         <v>23</v>
@@ -3589,10 +3589,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>26</v>
@@ -3601,7 +3601,7 @@
         <v>14</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G57" s="7" t="s">
         <v>23</v>
@@ -3622,10 +3622,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>21</v>
@@ -3655,10 +3655,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>181</v>
+        <v>329</v>
       </c>
       <c r="D59" s="12" t="s">
         <v>21</v>
@@ -3688,10 +3688,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>26</v>
@@ -3721,10 +3721,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>21</v>
@@ -3733,7 +3733,7 @@
         <v>14</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>23</v>
@@ -3754,10 +3754,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>26</v>
@@ -3766,7 +3766,7 @@
         <v>14</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>23</v>
@@ -3787,10 +3787,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>21</v>
@@ -3799,7 +3799,7 @@
         <v>14</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="G63" s="7" t="s">
         <v>23</v>
@@ -3820,10 +3820,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>21</v>
@@ -3832,7 +3832,7 @@
         <v>14</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="G64" s="7" t="s">
         <v>23</v>
@@ -3853,10 +3853,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>26</v>
@@ -3865,7 +3865,7 @@
         <v>14</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>23</v>
@@ -3886,10 +3886,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>199</v>
+        <v>330</v>
       </c>
       <c r="D66" s="18" t="s">
         <v>26</v>
@@ -3898,7 +3898,7 @@
         <v>14</v>
       </c>
       <c r="F66" s="25" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G66" s="8" t="s">
         <v>23</v>
@@ -3919,10 +3919,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>202</v>
+        <v>331</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>26</v>
@@ -3931,7 +3931,7 @@
         <v>14</v>
       </c>
       <c r="F67" s="25" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="G67" s="8" t="s">
         <v>23</v>
@@ -3940,13 +3940,13 @@
         <v>23</v>
       </c>
       <c r="I67" s="7" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="J67" s="8" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="K67" s="8" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
@@ -3954,10 +3954,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>208</v>
+        <v>332</v>
       </c>
       <c r="D68" s="18" t="s">
         <v>26</v>
@@ -3987,10 +3987,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>210</v>
+        <v>333</v>
       </c>
       <c r="D69" s="18" t="s">
         <v>26</v>
@@ -4020,10 +4020,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="D70" s="18" t="s">
         <v>26</v>
@@ -4053,10 +4053,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="D71" s="18" t="s">
         <v>26</v>
@@ -4086,10 +4086,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="D72" s="18" t="s">
         <v>26</v>
@@ -4119,10 +4119,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="D73" s="18" t="s">
         <v>26</v>
@@ -4152,10 +4152,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="D74" s="18" t="s">
         <v>26</v>
@@ -4185,10 +4185,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="D75" s="18" t="s">
         <v>26</v>
@@ -4218,10 +4218,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="42" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C76" s="43" t="s">
-        <v>224</v>
+        <v>334</v>
       </c>
       <c r="D76" s="18" t="s">
         <v>26</v>
@@ -4251,10 +4251,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="42" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C77" s="43" t="s">
-        <v>226</v>
+        <v>335</v>
       </c>
       <c r="D77" s="18" t="s">
         <v>26</v>
@@ -4284,10 +4284,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="40" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="C78" s="41" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="D78" s="18" t="s">
         <v>26</v>
@@ -4317,10 +4317,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="44" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C79" s="45" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="D79" s="18" t="s">
         <v>26</v>
@@ -4329,7 +4329,7 @@
         <v>14</v>
       </c>
       <c r="F79" s="25" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="G79" s="18" t="s">
         <v>23</v>
@@ -4350,10 +4350,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D80" s="18" t="s">
         <v>26</v>
@@ -4362,7 +4362,7 @@
         <v>14</v>
       </c>
       <c r="F80" s="25" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="G80" s="18" t="s">
         <v>23</v>
@@ -4383,10 +4383,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="D81" s="18" t="s">
         <v>26</v>
@@ -4395,7 +4395,7 @@
         <v>14</v>
       </c>
       <c r="F81" s="25" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="G81" s="18" t="s">
         <v>23</v>
@@ -4416,10 +4416,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="D82" s="18" t="s">
         <v>26</v>
@@ -4428,7 +4428,7 @@
         <v>14</v>
       </c>
       <c r="F82" s="25" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="G82" s="18" t="s">
         <v>23</v>
@@ -4449,10 +4449,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="D83" s="18" t="s">
         <v>26</v>
@@ -4461,7 +4461,7 @@
         <v>14</v>
       </c>
       <c r="F83" s="25" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G83" s="18" t="s">
         <v>23</v>
@@ -4482,10 +4482,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="D84" s="18" t="s">
         <v>26</v>
@@ -4494,7 +4494,7 @@
         <v>14</v>
       </c>
       <c r="F84" s="25" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="G84" s="18" t="s">
         <v>23</v>
@@ -4515,10 +4515,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="D85" s="18" t="s">
         <v>26</v>
@@ -4527,7 +4527,7 @@
         <v>14</v>
       </c>
       <c r="F85" s="25" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="G85" s="18" t="s">
         <v>23</v>
@@ -4548,10 +4548,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="18" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="D86" s="18" t="s">
         <v>26</v>
@@ -4560,7 +4560,7 @@
         <v>14</v>
       </c>
       <c r="F86" s="25" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="G86" s="18" t="s">
         <v>23</v>
@@ -4581,10 +4581,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="18" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="D87" s="18" t="s">
         <v>26</v>
@@ -4593,7 +4593,7 @@
         <v>14</v>
       </c>
       <c r="F87" s="25" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="G87" s="18" t="s">
         <v>23</v>
@@ -4614,10 +4614,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="D88" s="18" t="s">
         <v>26</v>
@@ -4626,7 +4626,7 @@
         <v>14</v>
       </c>
       <c r="F88" s="25" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="G88" s="18" t="s">
         <v>23</v>
@@ -4647,10 +4647,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="18" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="D89" s="18" t="s">
         <v>26</v>
@@ -4680,10 +4680,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="18" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="D90" s="18" t="s">
         <v>26</v>
@@ -4713,10 +4713,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="18" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="D91" s="18" t="s">
         <v>26</v>
@@ -4725,7 +4725,7 @@
         <v>14</v>
       </c>
       <c r="F91" s="27" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="G91" s="18" t="s">
         <v>23</v>
@@ -4746,10 +4746,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="18" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="D92" s="18" t="s">
         <v>26</v>
@@ -4758,7 +4758,7 @@
         <v>14</v>
       </c>
       <c r="F92" s="18" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="G92" s="18" t="s">
         <v>23</v>
@@ -4779,10 +4779,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="18" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="D93" s="18" t="s">
         <v>26</v>
@@ -4812,10 +4812,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="18" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>272</v>
+        <v>336</v>
       </c>
       <c r="D94" s="18" t="s">
         <v>26</v>
@@ -4845,10 +4845,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="18" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="D95" s="18" t="s">
         <v>26</v>
@@ -4857,7 +4857,7 @@
         <v>14</v>
       </c>
       <c r="F95" s="18" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="G95" s="18" t="s">
         <v>23</v>
@@ -4878,10 +4878,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="18" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="D96" s="18" t="s">
         <v>26</v>
@@ -4890,13 +4890,13 @@
         <v>14</v>
       </c>
       <c r="F96" s="18" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="G96" s="18" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="H96" s="18" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="I96" s="18"/>
       <c r="J96" s="18" t="s">
@@ -4911,10 +4911,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="28" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C97" s="29" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="D97" s="28" t="s">
         <v>26</v>
@@ -4923,22 +4923,22 @@
         <v>14</v>
       </c>
       <c r="F97" s="30" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="G97" s="28" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="H97" s="31" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="I97" s="32" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="J97" s="28" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="K97" s="28" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="98" spans="1:11" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4946,10 +4946,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="28" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="C98" s="33" t="s">
-        <v>289</v>
+        <v>337</v>
       </c>
       <c r="D98" s="28" t="s">
         <v>26</v>
@@ -4958,22 +4958,22 @@
         <v>14</v>
       </c>
       <c r="F98" s="28" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="G98" s="28" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="H98" s="28" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="I98" s="32" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="J98" s="28" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="K98" s="28" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="99" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -4981,10 +4981,10 @@
         <v>98</v>
       </c>
       <c r="B99" s="28" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="C99" s="33" t="s">
-        <v>294</v>
+        <v>338</v>
       </c>
       <c r="D99" s="28" t="s">
         <v>26</v>
@@ -4993,7 +4993,7 @@
         <v>14</v>
       </c>
       <c r="F99" s="34" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="G99" s="28" t="s">
         <v>23</v>
@@ -5002,10 +5002,10 @@
         <v>23</v>
       </c>
       <c r="I99" s="34" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="J99" s="28" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="K99" s="28" t="s">
         <v>18</v>
@@ -5016,10 +5016,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="28" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="C100" s="33" t="s">
-        <v>298</v>
+        <v>339</v>
       </c>
       <c r="D100" s="28" t="s">
         <v>26</v>
@@ -5028,22 +5028,22 @@
         <v>14</v>
       </c>
       <c r="F100" s="28" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
       <c r="G100" s="28" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="H100" s="28" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
       <c r="I100" s="32" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
       <c r="J100" s="28" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="K100" s="28" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="101" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -5051,10 +5051,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="28" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="C101" s="33" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="D101" s="28" t="s">
         <v>26</v>
@@ -5084,10 +5084,10 @@
         <v>101</v>
       </c>
       <c r="B102" s="28" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="C102" s="33" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="D102" s="28" t="s">
         <v>26</v>
@@ -5096,19 +5096,19 @@
         <v>14</v>
       </c>
       <c r="F102" s="32" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="G102" s="28" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="H102" s="32" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="I102" s="32" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="J102" s="28" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="K102" s="28" t="s">
         <v>48</v>
@@ -5119,10 +5119,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="28" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="C103" s="19" t="s">
-        <v>310</v>
+        <v>340</v>
       </c>
       <c r="D103" s="28" t="s">
         <v>26</v>
@@ -5131,7 +5131,7 @@
         <v>14</v>
       </c>
       <c r="F103" s="36" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="G103" s="28" t="s">
         <v>23</v>
@@ -5140,10 +5140,10 @@
         <v>23</v>
       </c>
       <c r="I103" s="36" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
       <c r="J103" s="28" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="K103" s="28" t="s">
         <v>18</v>
@@ -5154,10 +5154,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="28" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="C104" s="29" t="s">
-        <v>314</v>
+        <v>341</v>
       </c>
       <c r="D104" s="28" t="s">
         <v>26</v>
@@ -5166,22 +5166,22 @@
         <v>14</v>
       </c>
       <c r="F104" s="30" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="G104" s="28" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="H104" s="30" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="I104" s="32" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="J104" s="28" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="K104" s="28" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="105" spans="1:11" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -5189,10 +5189,10 @@
         <v>104</v>
       </c>
       <c r="B105" s="28" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="C105" s="33" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="D105" s="28" t="s">
         <v>26</v>
@@ -5201,22 +5201,22 @@
         <v>14</v>
       </c>
       <c r="F105" s="32" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="G105" s="28" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="H105" s="32" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="I105" s="37" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="J105" s="28" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="K105" s="28" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="106" spans="1:11" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -5224,10 +5224,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="28" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="C106" s="33" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="D106" s="28" t="s">
         <v>26</v>
@@ -5236,22 +5236,22 @@
         <v>14</v>
       </c>
       <c r="F106" s="32" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="G106" s="28" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="H106" s="32" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="I106" s="32" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="J106" s="28" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="K106" s="28" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="107" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -5259,10 +5259,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="28" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="C107" s="33" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="D107" s="28" t="s">
         <v>26</v>
@@ -5271,22 +5271,22 @@
         <v>14</v>
       </c>
       <c r="F107" s="28" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
       <c r="G107" s="28" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="H107" s="28" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="I107" s="37" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
       <c r="J107" s="28" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="K107" s="28" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="108" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -5294,10 +5294,10 @@
         <v>107</v>
       </c>
       <c r="B108" s="28" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="C108" s="33" t="s">
-        <v>334</v>
+        <v>316</v>
       </c>
       <c r="D108" s="28" t="s">
         <v>26</v>
@@ -5306,7 +5306,7 @@
         <v>14</v>
       </c>
       <c r="F108" s="34" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="G108" s="28" t="s">
         <v>23</v>
@@ -5315,10 +5315,10 @@
         <v>23</v>
       </c>
       <c r="I108" s="34" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="J108" s="28" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="K108" s="28" t="s">
         <v>18</v>
@@ -5329,10 +5329,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="C109" t="s">
-        <v>338</v>
+        <v>320</v>
       </c>
       <c r="D109" s="46" t="s">
         <v>21</v>
@@ -5341,16 +5341,16 @@
         <v>14</v>
       </c>
       <c r="F109" s="47" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>340</v>
+        <v>322</v>
       </c>
       <c r="H109">
         <v>5</v>
       </c>
       <c r="I109" s="46" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="J109" s="48" t="s">
         <v>17</v>
@@ -5439,8 +5439,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" topLeftCell="A2">
-      <selection activeCell="G12" sqref="G12"/>
+    <customSheetView guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" topLeftCell="A51">
+      <selection activeCell="G56" sqref="G56"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -5449,8 +5449,8 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" topLeftCell="A51">
-      <selection activeCell="G56" sqref="G56"/>
+    <customSheetView guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" topLeftCell="A2">
+      <selection activeCell="G12" sqref="G12"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -5461,12 +5461,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5711,21 +5714,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9BE38D0-BD1C-4126-A2D1-5A24E80B0CB5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6BB7CB2-3E08-455A-88BD-99593455AB98}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5750,12 +5753,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6BB7CB2-3E08-455A-88BD-99593455AB98}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9BE38D0-BD1C-4126-A2D1-5A24E80B0CB5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changes according to Tracys comments in github
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S1_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S1_P2.xlsx
@@ -16,9 +16,9 @@
   </sheets>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="Osei, Tracy Bonsu - Personal View" guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
+    <customWorkbookView name="Siampani, Sofia Maria - Personal View" guid="{D25176B6-2194-4D8F-99D6-14D593512471}" mergeInterval="0" personalView="1" xWindow="960" windowWidth="960" windowHeight="977" activeSheetId="1"/>
     <customWorkbookView name="49152 - Personal View" guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
-    <customWorkbookView name="Siampani, Sofia Maria - Personal View" guid="{D25176B6-2194-4D8F-99D6-14D593512471}" mergeInterval="0" personalView="1" xWindow="960" windowWidth="960" windowHeight="977" activeSheetId="1"/>
-    <customWorkbookView name="Osei, Tracy Bonsu - Personal View" guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="342">
   <si>
     <t>index</t>
   </si>
@@ -167,9 +167,6 @@
   </si>
   <si>
     <t>atcigsmk</t>
-  </si>
-  <si>
-    <t>tentive</t>
   </si>
   <si>
     <t>compatible</t>
@@ -1685,8 +1682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" topLeftCell="G23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2034,10 +2031,10 @@
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="12" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2045,10 +2042,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>48</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>49</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>26</v>
@@ -2070,7 +2067,7 @@
         <v>37</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2078,10 +2075,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>51</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>52</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>26</v>
@@ -2103,7 +2100,7 @@
         <v>37</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2111,31 +2108,31 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="D13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="11" t="s">
+      <c r="G13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="17" t="s">
+      <c r="J13" s="12" t="s">
         <v>56</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>57</v>
       </c>
       <c r="K13" s="12" t="s">
         <v>18</v>
@@ -2146,10 +2143,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>58</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>59</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>21</v>
@@ -2179,10 +2176,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>61</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>21</v>
@@ -2198,7 +2195,7 @@
         <v>37</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>37</v>
@@ -2212,10 +2209,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="16" t="s">
         <v>63</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>64</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>21</v>
@@ -2231,7 +2228,7 @@
         <v>37</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J16" s="12" t="s">
         <v>37</v>
@@ -2245,10 +2242,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>21</v>
@@ -2264,7 +2261,7 @@
         <v>37</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J17" s="12" t="s">
         <v>37</v>
@@ -2278,10 +2275,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>66</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>67</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>21</v>
@@ -2311,10 +2308,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>69</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>26</v>
@@ -2344,10 +2341,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>70</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>71</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>26</v>
@@ -2377,19 +2374,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="D21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="18" t="s">
         <v>73</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>74</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>23</v>
@@ -2410,10 +2407,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>75</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>76</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>26</v>
@@ -2443,19 +2440,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="D23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="18" t="s">
         <v>78</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>79</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>23</v>
@@ -2476,10 +2473,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>21</v>
@@ -2488,7 +2485,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>23</v>
@@ -2509,10 +2506,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="21" t="s">
         <v>82</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>83</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>21</v>
@@ -2521,7 +2518,7 @@
         <v>14</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>23</v>
@@ -2542,10 +2539,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>86</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>21</v>
@@ -2554,22 +2551,22 @@
         <v>14</v>
       </c>
       <c r="F26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>88</v>
       </c>
       <c r="J26" s="12" t="s">
         <v>17</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -2577,10 +2574,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>89</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>90</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>21</v>
@@ -2610,10 +2607,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="16" t="s">
         <v>91</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>92</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>21</v>
@@ -2622,19 +2619,19 @@
         <v>14</v>
       </c>
       <c r="F28" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="G28" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="I28" s="38" t="s">
-        <v>94</v>
-      </c>
       <c r="J28" s="12" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="K28" s="12" t="s">
         <v>18</v>
@@ -2645,10 +2642,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="16" t="s">
         <v>95</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>96</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>21</v>
@@ -2657,19 +2654,19 @@
         <v>14</v>
       </c>
       <c r="F29" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="G29" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="I29" s="39" t="s">
-        <v>98</v>
-      </c>
       <c r="J29" s="12" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="K29" s="12" t="s">
         <v>18</v>
@@ -2680,10 +2677,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="16" t="s">
         <v>99</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>100</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>21</v>
@@ -2692,19 +2689,19 @@
         <v>14</v>
       </c>
       <c r="F30" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I30" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="G30" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H30" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>102</v>
-      </c>
       <c r="J30" s="12" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>18</v>
@@ -2715,10 +2712,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="14" t="s">
         <v>103</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>104</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>21</v>
@@ -2728,7 +2725,7 @@
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>37</v>
@@ -2748,10 +2745,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>106</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>107</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>21</v>
@@ -2761,7 +2758,7 @@
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>37</v>
@@ -2781,10 +2778,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="14" t="s">
         <v>108</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>109</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>21</v>
@@ -2794,7 +2791,7 @@
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>37</v>
@@ -2803,7 +2800,7 @@
         <v>38</v>
       </c>
       <c r="J33" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K33" s="12" t="s">
         <v>38</v>
@@ -2814,10 +2811,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" s="14" t="s">
         <v>110</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>111</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>21</v>
@@ -2827,7 +2824,7 @@
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>37</v>
@@ -2847,10 +2844,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>21</v>
@@ -2860,7 +2857,7 @@
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H35" s="12" t="s">
         <v>37</v>
@@ -2880,10 +2877,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>21</v>
@@ -2893,7 +2890,7 @@
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H36" s="12" t="s">
         <v>37</v>
@@ -2913,10 +2910,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>21</v>
@@ -2926,7 +2923,7 @@
       </c>
       <c r="F37" s="12"/>
       <c r="G37" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H37" s="12" t="s">
         <v>37</v>
@@ -2946,10 +2943,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" s="14" t="s">
         <v>115</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>116</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>21</v>
@@ -2958,7 +2955,7 @@
         <v>14</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>23</v>
@@ -2979,10 +2976,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="14" t="s">
         <v>118</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>119</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>21</v>
@@ -2992,7 +2989,7 @@
       </c>
       <c r="F39" s="12"/>
       <c r="G39" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H39" s="12" t="s">
         <v>37</v>
@@ -3012,10 +3009,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="14" t="s">
         <v>120</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>121</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>21</v>
@@ -3025,7 +3022,7 @@
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H40" s="12" t="s">
         <v>37</v>
@@ -3045,10 +3042,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" s="14" t="s">
         <v>122</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>123</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>26</v>
@@ -3058,7 +3055,7 @@
       </c>
       <c r="F41" s="12"/>
       <c r="G41" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H41" s="12" t="s">
         <v>37</v>
@@ -3078,10 +3075,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C42" s="21" t="s">
         <v>124</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>125</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>21</v>
@@ -3091,7 +3088,7 @@
       </c>
       <c r="F42" s="12"/>
       <c r="G42" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H42" s="12" t="s">
         <v>37</v>
@@ -3111,10 +3108,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="13" t="s">
         <v>126</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>127</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>26</v>
@@ -3124,7 +3121,7 @@
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H43" s="7" t="s">
         <v>37</v>
@@ -3144,10 +3141,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" s="16" t="s">
         <v>128</v>
-      </c>
-      <c r="C44" s="16" t="s">
-        <v>129</v>
       </c>
       <c r="D44" s="12" t="s">
         <v>21</v>
@@ -3156,16 +3153,16 @@
         <v>14</v>
       </c>
       <c r="F44" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H44" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I44" s="14" t="s">
         <v>130</v>
-      </c>
-      <c r="G44" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H44" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="I44" s="14" t="s">
-        <v>131</v>
       </c>
       <c r="J44" s="12" t="s">
         <v>17</v>
@@ -3179,28 +3176,28 @@
         <v>44</v>
       </c>
       <c r="B45" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="D45" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F45" s="24" t="s">
+      <c r="G45" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I45" s="21" t="s">
         <v>134</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H45" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I45" s="21" t="s">
-        <v>135</v>
       </c>
       <c r="J45" s="12" t="s">
         <v>17</v>
@@ -3214,10 +3211,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>21</v>
@@ -3226,16 +3223,16 @@
         <v>14</v>
       </c>
       <c r="F46" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I46" s="24" t="s">
         <v>138</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H46" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I46" s="24" t="s">
-        <v>139</v>
       </c>
       <c r="J46" s="12" t="s">
         <v>17</v>
@@ -3249,28 +3246,28 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="D47" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F47" s="24" t="s">
+      <c r="G47" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I47" s="21" t="s">
         <v>142</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H47" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I47" s="21" t="s">
-        <v>143</v>
       </c>
       <c r="J47" s="7" t="s">
         <v>17</v>
@@ -3284,10 +3281,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C48" s="16" t="s">
         <v>144</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>145</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>21</v>
@@ -3296,16 +3293,16 @@
         <v>14</v>
       </c>
       <c r="F48" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I48" s="14" t="s">
         <v>146</v>
-      </c>
-      <c r="G48" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H48" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="I48" s="14" t="s">
-        <v>147</v>
       </c>
       <c r="J48" s="19" t="s">
         <v>17</v>
@@ -3319,28 +3316,28 @@
         <v>48</v>
       </c>
       <c r="B49" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C49" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="D49" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I49" s="13" t="s">
         <v>149</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F49" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H49" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I49" s="13" t="s">
-        <v>150</v>
       </c>
       <c r="J49" s="12" t="s">
         <v>17</v>
@@ -3354,10 +3351,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C50" s="16" t="s">
         <v>151</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>152</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>21</v>
@@ -3366,16 +3363,16 @@
         <v>14</v>
       </c>
       <c r="F50" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H50" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I50" s="14" t="s">
         <v>153</v>
-      </c>
-      <c r="G50" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H50" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="I50" s="14" t="s">
-        <v>154</v>
       </c>
       <c r="J50" s="12" t="s">
         <v>17</v>
@@ -3389,28 +3386,28 @@
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C51" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="D51" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H51" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I51" s="21" t="s">
         <v>156</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H51" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I51" s="21" t="s">
-        <v>157</v>
       </c>
       <c r="J51" s="12" t="s">
         <v>17</v>
@@ -3424,10 +3421,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C52" s="16" t="s">
         <v>158</v>
-      </c>
-      <c r="C52" s="16" t="s">
-        <v>159</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>21</v>
@@ -3437,7 +3434,7 @@
       </c>
       <c r="F52" s="12"/>
       <c r="G52" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H52" s="12" t="s">
         <v>37</v>
@@ -3457,10 +3454,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C53" s="16" t="s">
         <v>160</v>
-      </c>
-      <c r="C53" s="16" t="s">
-        <v>161</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>26</v>
@@ -3470,7 +3467,7 @@
       </c>
       <c r="F53" s="12"/>
       <c r="G53" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H53" s="12" t="s">
         <v>37</v>
@@ -3490,10 +3487,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C54" s="14" t="s">
         <v>162</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>163</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>21</v>
@@ -3503,7 +3500,7 @@
       </c>
       <c r="F54" s="12"/>
       <c r="G54" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H54" s="12" t="s">
         <v>37</v>
@@ -3523,10 +3520,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="16" t="s">
         <v>164</v>
-      </c>
-      <c r="C55" s="16" t="s">
-        <v>165</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>26</v>
@@ -3536,7 +3533,7 @@
       </c>
       <c r="F55" s="12"/>
       <c r="G55" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H55" s="12" t="s">
         <v>37</v>
@@ -3556,10 +3553,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C56" s="16" t="s">
         <v>166</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>167</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>21</v>
@@ -3568,7 +3565,7 @@
         <v>14</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G56" s="7" t="s">
         <v>23</v>
@@ -3589,19 +3586,19 @@
         <v>56</v>
       </c>
       <c r="B57" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C57" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="D57" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F57" s="24" t="s">
         <v>170</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F57" s="24" t="s">
-        <v>171</v>
       </c>
       <c r="G57" s="7" t="s">
         <v>23</v>
@@ -3622,10 +3619,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C58" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="C58" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>21</v>
@@ -3655,10 +3652,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D59" s="12" t="s">
         <v>21</v>
@@ -3688,10 +3685,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C60" s="14" t="s">
         <v>175</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>176</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>26</v>
@@ -3721,10 +3718,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C61" s="16" t="s">
         <v>177</v>
-      </c>
-      <c r="C61" s="16" t="s">
-        <v>178</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>21</v>
@@ -3733,7 +3730,7 @@
         <v>14</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>23</v>
@@ -3754,19 +3751,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C62" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="D62" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F62" s="24" t="s">
         <v>181</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F62" s="24" t="s">
-        <v>182</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>23</v>
@@ -3787,10 +3784,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C63" s="16" t="s">
         <v>183</v>
-      </c>
-      <c r="C63" s="16" t="s">
-        <v>184</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>21</v>
@@ -3799,7 +3796,7 @@
         <v>14</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G63" s="7" t="s">
         <v>23</v>
@@ -3820,10 +3817,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C64" s="14" t="s">
         <v>186</v>
-      </c>
-      <c r="C64" s="14" t="s">
-        <v>187</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>21</v>
@@ -3832,7 +3829,7 @@
         <v>14</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G64" s="7" t="s">
         <v>23</v>
@@ -3853,11 +3850,11 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C65" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="C65" s="14" t="s">
-        <v>190</v>
-      </c>
       <c r="D65" s="7" t="s">
         <v>26</v>
       </c>
@@ -3865,7 +3862,7 @@
         <v>14</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>23</v>
@@ -3886,19 +3883,19 @@
         <v>65</v>
       </c>
       <c r="B66" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F66" s="25" t="s">
         <v>191</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>328</v>
-      </c>
-      <c r="D66" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E66" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F66" s="25" t="s">
-        <v>192</v>
       </c>
       <c r="G66" s="8" t="s">
         <v>23</v>
@@ -3919,34 +3916,34 @@
         <v>66</v>
       </c>
       <c r="B67" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="C67" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="D67" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F67" s="25" t="s">
+      <c r="G67" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I67" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="G67" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H67" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I67" s="7" t="s">
+      <c r="J67" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="J67" s="8" t="s">
+      <c r="K67" s="8" t="s">
         <v>196</v>
-      </c>
-      <c r="K67" s="8" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
@@ -3954,10 +3951,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D68" s="18" t="s">
         <v>26</v>
@@ -3987,10 +3984,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D69" s="18" t="s">
         <v>26</v>
@@ -4020,10 +4017,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="C70" s="12" t="s">
         <v>200</v>
-      </c>
-      <c r="C70" s="12" t="s">
-        <v>201</v>
       </c>
       <c r="D70" s="18" t="s">
         <v>26</v>
@@ -4053,10 +4050,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="C71" s="12" t="s">
         <v>202</v>
-      </c>
-      <c r="C71" s="12" t="s">
-        <v>203</v>
       </c>
       <c r="D71" s="18" t="s">
         <v>26</v>
@@ -4086,10 +4083,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="C72" s="12" t="s">
         <v>204</v>
-      </c>
-      <c r="C72" s="12" t="s">
-        <v>205</v>
       </c>
       <c r="D72" s="18" t="s">
         <v>26</v>
@@ -4119,10 +4116,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="C73" s="12" t="s">
         <v>206</v>
-      </c>
-      <c r="C73" s="12" t="s">
-        <v>207</v>
       </c>
       <c r="D73" s="18" t="s">
         <v>26</v>
@@ -4152,10 +4149,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="C74" s="12" t="s">
         <v>208</v>
-      </c>
-      <c r="C74" s="12" t="s">
-        <v>209</v>
       </c>
       <c r="D74" s="18" t="s">
         <v>26</v>
@@ -4185,10 +4182,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="C75" s="12" t="s">
         <v>210</v>
-      </c>
-      <c r="C75" s="12" t="s">
-        <v>211</v>
       </c>
       <c r="D75" s="18" t="s">
         <v>26</v>
@@ -4218,10 +4215,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C76" s="43" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D76" s="18" t="s">
         <v>26</v>
@@ -4251,10 +4248,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C77" s="43" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D77" s="18" t="s">
         <v>26</v>
@@ -4284,10 +4281,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="40" t="s">
+        <v>213</v>
+      </c>
+      <c r="C78" s="41" t="s">
         <v>214</v>
-      </c>
-      <c r="C78" s="41" t="s">
-        <v>215</v>
       </c>
       <c r="D78" s="18" t="s">
         <v>26</v>
@@ -4317,19 +4314,19 @@
         <v>78</v>
       </c>
       <c r="B79" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="C79" s="45" t="s">
         <v>216</v>
       </c>
-      <c r="C79" s="45" t="s">
+      <c r="D79" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E79" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79" s="25" t="s">
         <v>217</v>
-      </c>
-      <c r="D79" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E79" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F79" s="25" t="s">
-        <v>218</v>
       </c>
       <c r="G79" s="18" t="s">
         <v>23</v>
@@ -4350,19 +4347,19 @@
         <v>79</v>
       </c>
       <c r="B80" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="C80" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="C80" s="12" t="s">
+      <c r="D80" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80" s="25" t="s">
         <v>220</v>
-      </c>
-      <c r="D80" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F80" s="25" t="s">
-        <v>221</v>
       </c>
       <c r="G80" s="18" t="s">
         <v>23</v>
@@ -4383,19 +4380,19 @@
         <v>80</v>
       </c>
       <c r="B81" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="C81" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="C81" s="12" t="s">
+      <c r="D81" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" s="25" t="s">
         <v>223</v>
-      </c>
-      <c r="D81" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F81" s="25" t="s">
-        <v>224</v>
       </c>
       <c r="G81" s="18" t="s">
         <v>23</v>
@@ -4416,19 +4413,19 @@
         <v>81</v>
       </c>
       <c r="B82" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="C82" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="C82" s="12" t="s">
+      <c r="D82" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F82" s="25" t="s">
         <v>226</v>
-      </c>
-      <c r="D82" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F82" s="25" t="s">
-        <v>227</v>
       </c>
       <c r="G82" s="18" t="s">
         <v>23</v>
@@ -4449,19 +4446,19 @@
         <v>82</v>
       </c>
       <c r="B83" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="C83" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="C83" s="12" t="s">
+      <c r="D83" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83" s="25" t="s">
         <v>229</v>
-      </c>
-      <c r="D83" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E83" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F83" s="25" t="s">
-        <v>230</v>
       </c>
       <c r="G83" s="18" t="s">
         <v>23</v>
@@ -4482,19 +4479,19 @@
         <v>83</v>
       </c>
       <c r="B84" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="C84" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="C84" s="12" t="s">
+      <c r="D84" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" s="25" t="s">
         <v>232</v>
-      </c>
-      <c r="D84" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E84" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F84" s="25" t="s">
-        <v>233</v>
       </c>
       <c r="G84" s="18" t="s">
         <v>23</v>
@@ -4515,19 +4512,19 @@
         <v>84</v>
       </c>
       <c r="B85" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="C85" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="C85" s="12" t="s">
+      <c r="D85" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="25" t="s">
         <v>235</v>
-      </c>
-      <c r="D85" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E85" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F85" s="25" t="s">
-        <v>236</v>
       </c>
       <c r="G85" s="18" t="s">
         <v>23</v>
@@ -4548,19 +4545,19 @@
         <v>85</v>
       </c>
       <c r="B86" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="C86" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="C86" s="12" t="s">
+      <c r="D86" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F86" s="25" t="s">
         <v>238</v>
-      </c>
-      <c r="D86" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F86" s="25" t="s">
-        <v>239</v>
       </c>
       <c r="G86" s="18" t="s">
         <v>23</v>
@@ -4581,19 +4578,19 @@
         <v>86</v>
       </c>
       <c r="B87" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="C87" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="C87" s="12" t="s">
+      <c r="D87" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F87" s="25" t="s">
         <v>241</v>
-      </c>
-      <c r="D87" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F87" s="25" t="s">
-        <v>242</v>
       </c>
       <c r="G87" s="18" t="s">
         <v>23</v>
@@ -4614,11 +4611,11 @@
         <v>87</v>
       </c>
       <c r="B88" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="C88" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="C88" s="12" t="s">
-        <v>244</v>
-      </c>
       <c r="D88" s="18" t="s">
         <v>26</v>
       </c>
@@ -4626,22 +4623,22 @@
         <v>14</v>
       </c>
       <c r="F88" s="25" t="s">
+        <v>340</v>
+      </c>
+      <c r="G88" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="H88" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="I88" s="18" t="s">
         <v>341</v>
-      </c>
-      <c r="G88" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="H88" s="18" t="s">
-        <v>340</v>
-      </c>
-      <c r="I88" s="18" t="s">
-        <v>342</v>
       </c>
       <c r="J88" s="18" t="s">
         <v>17</v>
       </c>
       <c r="K88" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.35">
@@ -4649,10 +4646,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="C89" s="12" t="s">
         <v>245</v>
-      </c>
-      <c r="C89" s="12" t="s">
-        <v>246</v>
       </c>
       <c r="D89" s="18" t="s">
         <v>26</v>
@@ -4682,10 +4679,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="C90" s="12" t="s">
         <v>247</v>
-      </c>
-      <c r="C90" s="12" t="s">
-        <v>248</v>
       </c>
       <c r="D90" s="18" t="s">
         <v>26</v>
@@ -4715,19 +4712,19 @@
         <v>90</v>
       </c>
       <c r="B91" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="C91" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="C91" s="12" t="s">
+      <c r="D91" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F91" s="27" t="s">
         <v>250</v>
-      </c>
-      <c r="D91" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E91" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F91" s="27" t="s">
-        <v>251</v>
       </c>
       <c r="G91" s="18" t="s">
         <v>23</v>
@@ -4748,19 +4745,19 @@
         <v>91</v>
       </c>
       <c r="B92" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="C92" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="C92" s="12" t="s">
+      <c r="D92" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F92" s="18" t="s">
         <v>253</v>
-      </c>
-      <c r="D92" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E92" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F92" s="18" t="s">
-        <v>254</v>
       </c>
       <c r="G92" s="18" t="s">
         <v>23</v>
@@ -4781,10 +4778,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="C93" s="12" t="s">
         <v>255</v>
-      </c>
-      <c r="C93" s="12" t="s">
-        <v>256</v>
       </c>
       <c r="D93" s="18" t="s">
         <v>26</v>
@@ -4814,10 +4811,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D94" s="18" t="s">
         <v>26</v>
@@ -4847,19 +4844,19 @@
         <v>94</v>
       </c>
       <c r="B95" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="C95" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="C95" s="12" t="s">
+      <c r="D95" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F95" s="18" t="s">
         <v>259</v>
-      </c>
-      <c r="D95" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F95" s="18" t="s">
-        <v>260</v>
       </c>
       <c r="G95" s="18" t="s">
         <v>23</v>
@@ -4880,25 +4877,25 @@
         <v>95</v>
       </c>
       <c r="B96" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="C96" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="C96" s="12" t="s">
+      <c r="D96" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F96" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="D96" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F96" s="18" t="s">
+      <c r="G96" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="G96" s="18" t="s">
+      <c r="H96" s="18" t="s">
         <v>264</v>
-      </c>
-      <c r="H96" s="18" t="s">
-        <v>265</v>
       </c>
       <c r="I96" s="18"/>
       <c r="J96" s="18" t="s">
@@ -4913,34 +4910,34 @@
         <v>96</v>
       </c>
       <c r="B97" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="C97" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="C97" s="29" t="s">
+      <c r="D97" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E97" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F97" s="30" t="s">
         <v>267</v>
       </c>
-      <c r="D97" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E97" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F97" s="30" t="s">
+      <c r="G97" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="H97" s="31" t="s">
         <v>268</v>
       </c>
-      <c r="G97" s="28" t="s">
-        <v>264</v>
-      </c>
-      <c r="H97" s="31" t="s">
+      <c r="I97" s="32" t="s">
         <v>269</v>
       </c>
-      <c r="I97" s="32" t="s">
+      <c r="J97" s="28" t="s">
         <v>270</v>
       </c>
-      <c r="J97" s="28" t="s">
+      <c r="K97" s="28" t="s">
         <v>271</v>
-      </c>
-      <c r="K97" s="28" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="98" spans="1:11" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -4948,34 +4945,34 @@
         <v>97</v>
       </c>
       <c r="B98" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="C98" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="D98" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E98" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F98" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="C98" s="33" t="s">
-        <v>335</v>
-      </c>
-      <c r="D98" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E98" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F98" s="28" t="s">
+      <c r="G98" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="H98" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="G98" s="28" t="s">
-        <v>264</v>
-      </c>
-      <c r="H98" s="28" t="s">
+      <c r="I98" s="32" t="s">
         <v>275</v>
       </c>
-      <c r="I98" s="32" t="s">
-        <v>276</v>
-      </c>
       <c r="J98" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="K98" s="28" t="s">
         <v>271</v>
-      </c>
-      <c r="K98" s="28" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="99" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -4983,31 +4980,31 @@
         <v>98</v>
       </c>
       <c r="B99" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="C99" s="33" t="s">
+        <v>335</v>
+      </c>
+      <c r="D99" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E99" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F99" s="34" t="s">
         <v>277</v>
       </c>
-      <c r="C99" s="33" t="s">
-        <v>336</v>
-      </c>
-      <c r="D99" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E99" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F99" s="34" t="s">
+      <c r="G99" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H99" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="I99" s="34" t="s">
         <v>278</v>
       </c>
-      <c r="G99" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="H99" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="I99" s="34" t="s">
-        <v>279</v>
-      </c>
       <c r="J99" s="28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K99" s="28" t="s">
         <v>18</v>
@@ -5018,34 +5015,34 @@
         <v>99</v>
       </c>
       <c r="B100" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="C100" s="33" t="s">
+        <v>336</v>
+      </c>
+      <c r="D100" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E100" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100" s="28" t="s">
         <v>280</v>
       </c>
-      <c r="C100" s="33" t="s">
-        <v>337</v>
-      </c>
-      <c r="D100" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E100" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F100" s="28" t="s">
+      <c r="G100" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="H100" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="G100" s="28" t="s">
-        <v>264</v>
-      </c>
-      <c r="H100" s="28" t="s">
+      <c r="I100" s="32" t="s">
         <v>282</v>
       </c>
-      <c r="I100" s="32" t="s">
-        <v>283</v>
-      </c>
       <c r="J100" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="K100" s="28" t="s">
         <v>271</v>
-      </c>
-      <c r="K100" s="28" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="101" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -5053,10 +5050,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="C101" s="33" t="s">
         <v>284</v>
-      </c>
-      <c r="C101" s="33" t="s">
-        <v>285</v>
       </c>
       <c r="D101" s="28" t="s">
         <v>26</v>
@@ -5086,34 +5083,34 @@
         <v>101</v>
       </c>
       <c r="B102" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="C102" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="C102" s="33" t="s">
+      <c r="D102" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E102" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F102" s="32" t="s">
         <v>287</v>
       </c>
-      <c r="D102" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E102" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F102" s="32" t="s">
+      <c r="G102" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="H102" s="32" t="s">
         <v>288</v>
       </c>
-      <c r="G102" s="28" t="s">
-        <v>264</v>
-      </c>
-      <c r="H102" s="32" t="s">
+      <c r="I102" s="32" t="s">
         <v>289</v>
       </c>
-      <c r="I102" s="32" t="s">
-        <v>290</v>
-      </c>
       <c r="J102" s="28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K102" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="103" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -5121,31 +5118,31 @@
         <v>102</v>
       </c>
       <c r="B103" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="C103" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="D103" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E103" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F103" s="36" t="s">
         <v>291</v>
       </c>
-      <c r="C103" s="19" t="s">
-        <v>338</v>
-      </c>
-      <c r="D103" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E103" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F103" s="36" t="s">
+      <c r="G103" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H103" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I103" s="36" t="s">
         <v>292</v>
       </c>
-      <c r="G103" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="H103" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="I103" s="36" t="s">
-        <v>293</v>
-      </c>
       <c r="J103" s="28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K103" s="28" t="s">
         <v>18</v>
@@ -5156,34 +5153,34 @@
         <v>103</v>
       </c>
       <c r="B104" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="C104" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="D104" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E104" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F104" s="30" t="s">
         <v>294</v>
       </c>
-      <c r="C104" s="29" t="s">
-        <v>339</v>
-      </c>
-      <c r="D104" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E104" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F104" s="30" t="s">
+      <c r="G104" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="H104" s="30" t="s">
         <v>295</v>
       </c>
-      <c r="G104" s="28" t="s">
-        <v>264</v>
-      </c>
-      <c r="H104" s="30" t="s">
+      <c r="I104" s="32" t="s">
         <v>296</v>
       </c>
-      <c r="I104" s="32" t="s">
-        <v>297</v>
-      </c>
       <c r="J104" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="K104" s="28" t="s">
         <v>271</v>
-      </c>
-      <c r="K104" s="28" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="105" spans="1:11" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -5191,34 +5188,34 @@
         <v>104</v>
       </c>
       <c r="B105" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="C105" s="33" t="s">
         <v>298</v>
       </c>
-      <c r="C105" s="33" t="s">
+      <c r="D105" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E105" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F105" s="32" t="s">
         <v>299</v>
       </c>
-      <c r="D105" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E105" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F105" s="32" t="s">
+      <c r="G105" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="H105" s="32" t="s">
         <v>300</v>
       </c>
-      <c r="G105" s="28" t="s">
-        <v>264</v>
-      </c>
-      <c r="H105" s="32" t="s">
+      <c r="I105" s="37" t="s">
         <v>301</v>
       </c>
-      <c r="I105" s="37" t="s">
-        <v>302</v>
-      </c>
       <c r="J105" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="K105" s="28" t="s">
         <v>271</v>
-      </c>
-      <c r="K105" s="28" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="106" spans="1:11" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -5226,34 +5223,34 @@
         <v>105</v>
       </c>
       <c r="B106" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="C106" s="33" t="s">
         <v>303</v>
       </c>
-      <c r="C106" s="33" t="s">
+      <c r="D106" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E106" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F106" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="D106" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E106" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F106" s="32" t="s">
+      <c r="G106" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="H106" s="32" t="s">
         <v>305</v>
       </c>
-      <c r="G106" s="28" t="s">
-        <v>264</v>
-      </c>
-      <c r="H106" s="32" t="s">
+      <c r="I106" s="32" t="s">
         <v>306</v>
       </c>
-      <c r="I106" s="32" t="s">
-        <v>307</v>
-      </c>
       <c r="J106" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="K106" s="28" t="s">
         <v>271</v>
-      </c>
-      <c r="K106" s="28" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="107" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -5261,34 +5258,34 @@
         <v>106</v>
       </c>
       <c r="B107" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="C107" s="33" t="s">
         <v>308</v>
       </c>
-      <c r="C107" s="33" t="s">
+      <c r="D107" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E107" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F107" s="28" t="s">
         <v>309</v>
       </c>
-      <c r="D107" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E107" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F107" s="28" t="s">
+      <c r="G107" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="H107" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="G107" s="28" t="s">
-        <v>264</v>
-      </c>
-      <c r="H107" s="28" t="s">
+      <c r="I107" s="37" t="s">
         <v>311</v>
       </c>
-      <c r="I107" s="37" t="s">
-        <v>312</v>
-      </c>
       <c r="J107" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="K107" s="28" t="s">
         <v>271</v>
-      </c>
-      <c r="K107" s="28" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="108" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -5296,31 +5293,31 @@
         <v>107</v>
       </c>
       <c r="B108" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="C108" s="33" t="s">
         <v>313</v>
       </c>
-      <c r="C108" s="33" t="s">
+      <c r="D108" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E108" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F108" s="34" t="s">
         <v>314</v>
       </c>
-      <c r="D108" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E108" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F108" s="34" t="s">
+      <c r="G108" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H108" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="I108" s="34" t="s">
         <v>315</v>
       </c>
-      <c r="G108" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="H108" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="I108" s="34" t="s">
-        <v>316</v>
-      </c>
       <c r="J108" s="28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K108" s="28" t="s">
         <v>18</v>
@@ -5331,10 +5328,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
+        <v>316</v>
+      </c>
+      <c r="C109" t="s">
         <v>317</v>
-      </c>
-      <c r="C109" t="s">
-        <v>318</v>
       </c>
       <c r="D109" s="46" t="s">
         <v>21</v>
@@ -5343,16 +5340,16 @@
         <v>14</v>
       </c>
       <c r="F109" s="47" t="s">
+        <v>318</v>
+      </c>
+      <c r="G109" s="4" t="s">
         <v>319</v>
-      </c>
-      <c r="G109" s="4" t="s">
-        <v>320</v>
       </c>
       <c r="H109">
         <v>5</v>
       </c>
       <c r="I109" s="46" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J109" s="48" t="s">
         <v>17</v>
@@ -5441,8 +5438,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" topLeftCell="A2">
-      <selection activeCell="G12" sqref="G12"/>
+    <customSheetView guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" topLeftCell="A51">
+      <selection activeCell="G56" sqref="G56"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -5451,8 +5448,8 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" topLeftCell="A51">
-      <selection activeCell="G56" sqref="G56"/>
+    <customSheetView guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" topLeftCell="A2">
+      <selection activeCell="G12" sqref="G12"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -5463,6 +5460,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -5472,15 +5478,6 @@
     <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5725,20 +5722,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9BE38D0-BD1C-4126-A2D1-5A24E80B0CB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6BB7CB2-3E08-455A-88BD-99593455AB98}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
     <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9BE38D0-BD1C-4126-A2D1-5A24E80B0CB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
KORA S1- Unit of changed to mg/day and sodium potassium ratio unit taking away KORA S3-unit changed from g/day to mg/day and the unit of sodium patassium taking off.
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S1_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S1_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB57DD3-E750-4E9A-8336-D7CC8674E9B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3AB127-AB3B-46D9-8BB8-E31C6D032EF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20745" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,9 @@
   </sheets>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="49152 - Personal View" guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
+    <customWorkbookView name="Siampani, Sofia Maria - Personal View" guid="{D25176B6-2194-4D8F-99D6-14D593512471}" mergeInterval="0" personalView="1" xWindow="960" windowWidth="960" windowHeight="977" activeSheetId="1"/>
     <customWorkbookView name="Osei, Tracy Bonsu - Personal View" guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
-    <customWorkbookView name="Siampani, Sofia Maria - Personal View" guid="{D25176B6-2194-4D8F-99D6-14D593512471}" mergeInterval="0" personalView="1" xWindow="960" windowWidth="960" windowHeight="977" activeSheetId="1"/>
-    <customWorkbookView name="49152 - Personal View" guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -710,16 +710,10 @@
     <t>SODIUM</t>
   </si>
   <si>
-    <t>Sodium intake [g/d]</t>
-  </si>
-  <si>
     <t>anatr</t>
   </si>
   <si>
     <t>SOD_POT_RATIO</t>
-  </si>
-  <si>
-    <t>Sodium to potassium intake ratio [g/d]</t>
   </si>
   <si>
     <t>anatr; akal</t>
@@ -1094,6 +1088,12 @@
   </si>
   <si>
     <t>double the amount of AV491 (dry legumes) to be comparable to other studies</t>
+  </si>
+  <si>
+    <t>Sodium intake [mg/d]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sodium to potassium intake ratio </t>
   </si>
 </sst>
 </file>
@@ -1673,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H102" sqref="H102"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,7 +1803,7 @@
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
@@ -1937,7 +1937,7 @@
         <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
@@ -1970,7 +1970,7 @@
         <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
@@ -2036,7 +2036,7 @@
         <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D11" t="s">
         <v>24</v>
@@ -2069,7 +2069,7 @@
         <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D12" t="s">
         <v>24</v>
@@ -2102,7 +2102,7 @@
         <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D13" t="s">
         <v>24</v>
@@ -2236,7 +2236,7 @@
         <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
@@ -2269,7 +2269,7 @@
         <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -2302,7 +2302,7 @@
         <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D19" t="s">
         <v>24</v>
@@ -2335,7 +2335,7 @@
         <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>
@@ -2368,7 +2368,7 @@
         <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D21" t="s">
         <v>24</v>
@@ -2401,7 +2401,7 @@
         <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D22" t="s">
         <v>24</v>
@@ -2434,7 +2434,7 @@
         <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D23" t="s">
         <v>24</v>
@@ -2467,7 +2467,7 @@
         <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D24" t="s">
         <v>20</v>
@@ -2838,7 +2838,7 @@
         <v>98</v>
       </c>
       <c r="C35" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D35" t="s">
         <v>20</v>
@@ -2871,7 +2871,7 @@
         <v>99</v>
       </c>
       <c r="C36" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D36" t="s">
         <v>20</v>
@@ -2904,7 +2904,7 @@
         <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D37" t="s">
         <v>20</v>
@@ -3036,7 +3036,7 @@
         <v>108</v>
       </c>
       <c r="C41" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D41" t="s">
         <v>24</v>
@@ -3102,7 +3102,7 @@
         <v>111</v>
       </c>
       <c r="C43" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D43" t="s">
         <v>24</v>
@@ -3170,7 +3170,7 @@
         <v>116</v>
       </c>
       <c r="C45" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D45" t="s">
         <v>24</v>
@@ -3240,7 +3240,7 @@
         <v>123</v>
       </c>
       <c r="C47" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D47" t="s">
         <v>24</v>
@@ -3310,7 +3310,7 @@
         <v>130</v>
       </c>
       <c r="C49" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D49" t="s">
         <v>24</v>
@@ -3380,7 +3380,7 @@
         <v>136</v>
       </c>
       <c r="C51" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D51" t="s">
         <v>24</v>
@@ -3448,7 +3448,7 @@
         <v>140</v>
       </c>
       <c r="C53" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D53" t="s">
         <v>24</v>
@@ -3514,7 +3514,7 @@
         <v>143</v>
       </c>
       <c r="C55" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D55" t="s">
         <v>24</v>
@@ -3580,7 +3580,7 @@
         <v>147</v>
       </c>
       <c r="C57" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D57" t="s">
         <v>24</v>
@@ -3646,10 +3646,10 @@
         <v>151</v>
       </c>
       <c r="C59" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D59" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>13</v>
@@ -3679,7 +3679,7 @@
         <v>152</v>
       </c>
       <c r="C60" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D60" t="s">
         <v>24</v>
@@ -3745,7 +3745,7 @@
         <v>156</v>
       </c>
       <c r="C62" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D62" t="s">
         <v>24</v>
@@ -3844,7 +3844,7 @@
         <v>164</v>
       </c>
       <c r="C65" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D65" t="s">
         <v>24</v>
@@ -3877,7 +3877,7 @@
         <v>165</v>
       </c>
       <c r="C66" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D66" t="s">
         <v>24</v>
@@ -3910,7 +3910,7 @@
         <v>167</v>
       </c>
       <c r="C67" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D67" t="s">
         <v>24</v>
@@ -3945,7 +3945,7 @@
         <v>172</v>
       </c>
       <c r="C68" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D68" t="s">
         <v>24</v>
@@ -3978,7 +3978,7 @@
         <v>173</v>
       </c>
       <c r="C69" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D69" t="s">
         <v>24</v>
@@ -4011,7 +4011,7 @@
         <v>174</v>
       </c>
       <c r="C70" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D70" t="s">
         <v>24</v>
@@ -4044,7 +4044,7 @@
         <v>175</v>
       </c>
       <c r="C71" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D71" t="s">
         <v>24</v>
@@ -4077,7 +4077,7 @@
         <v>176</v>
       </c>
       <c r="C72" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D72" t="s">
         <v>24</v>
@@ -4110,7 +4110,7 @@
         <v>177</v>
       </c>
       <c r="C73" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D73" t="s">
         <v>24</v>
@@ -4143,7 +4143,7 @@
         <v>178</v>
       </c>
       <c r="C74" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D74" t="s">
         <v>24</v>
@@ -4176,7 +4176,7 @@
         <v>179</v>
       </c>
       <c r="C75" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D75" t="s">
         <v>24</v>
@@ -4209,7 +4209,7 @@
         <v>180</v>
       </c>
       <c r="C76" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D76" t="s">
         <v>24</v>
@@ -4242,7 +4242,7 @@
         <v>181</v>
       </c>
       <c r="C77" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D77" t="s">
         <v>24</v>
@@ -4275,7 +4275,7 @@
         <v>182</v>
       </c>
       <c r="C78" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D78" t="s">
         <v>24</v>
@@ -4614,16 +4614,16 @@
         <v>13</v>
       </c>
       <c r="F88" s="25" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G88" s="18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H88" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="I88" s="18" t="s">
         <v>300</v>
-      </c>
-      <c r="I88" s="18" t="s">
-        <v>302</v>
       </c>
       <c r="J88" s="18" t="s">
         <v>16</v>
@@ -4805,7 +4805,7 @@
         <v>224</v>
       </c>
       <c r="C94" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D94" t="s">
         <v>24</v>
@@ -4838,16 +4838,16 @@
         <v>225</v>
       </c>
       <c r="C95" t="s">
+        <v>341</v>
+      </c>
+      <c r="D95" t="s">
+        <v>24</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F95" s="18" t="s">
         <v>226</v>
-      </c>
-      <c r="D95" t="s">
-        <v>24</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F95" s="18" t="s">
-        <v>227</v>
       </c>
       <c r="G95" s="18" t="s">
         <v>22</v>
@@ -4868,25 +4868,25 @@
         <v>95</v>
       </c>
       <c r="B96" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="C96" t="s">
+        <v>342</v>
+      </c>
+      <c r="D96" t="s">
+        <v>24</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="C96" t="s">
+      <c r="G96" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="D96" t="s">
-        <v>24</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F96" s="18" t="s">
+      <c r="H96" s="18" t="s">
         <v>230</v>
-      </c>
-      <c r="G96" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="H96" s="18" t="s">
-        <v>232</v>
       </c>
       <c r="I96" s="18"/>
       <c r="J96" s="18" t="s">
@@ -4901,34 +4901,34 @@
         <v>96</v>
       </c>
       <c r="B97" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="C97" t="s">
+        <v>232</v>
+      </c>
+      <c r="D97" t="s">
+        <v>24</v>
+      </c>
+      <c r="E97" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F97" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="C97" t="s">
+      <c r="G97" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="H97" s="30" t="s">
         <v>234</v>
       </c>
-      <c r="D97" t="s">
-        <v>24</v>
-      </c>
-      <c r="E97" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F97" s="29" t="s">
+      <c r="I97" s="31" t="s">
         <v>235</v>
       </c>
-      <c r="G97" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="H97" s="30" t="s">
+      <c r="J97" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="I97" s="31" t="s">
+      <c r="K97" s="28" t="s">
         <v>237</v>
-      </c>
-      <c r="J97" s="28" t="s">
-        <v>238</v>
-      </c>
-      <c r="K97" s="28" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="98" spans="1:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4936,34 +4936,34 @@
         <v>97</v>
       </c>
       <c r="B98" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="C98" t="s">
+        <v>293</v>
+      </c>
+      <c r="D98" t="s">
+        <v>24</v>
+      </c>
+      <c r="E98" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F98" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="G98" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="H98" s="28" t="s">
         <v>240</v>
       </c>
-      <c r="C98" t="s">
-        <v>295</v>
-      </c>
-      <c r="D98" t="s">
-        <v>24</v>
-      </c>
-      <c r="E98" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F98" s="28" t="s">
+      <c r="I98" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="G98" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="H98" s="28" t="s">
-        <v>242</v>
-      </c>
-      <c r="I98" s="31" t="s">
-        <v>243</v>
-      </c>
       <c r="J98" s="28" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K98" s="28" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="99" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -4971,31 +4971,31 @@
         <v>98</v>
       </c>
       <c r="B99" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="C99" t="s">
+        <v>294</v>
+      </c>
+      <c r="D99" t="s">
+        <v>24</v>
+      </c>
+      <c r="E99" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F99" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="G99" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H99" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="I99" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="C99" t="s">
-        <v>296</v>
-      </c>
-      <c r="D99" t="s">
-        <v>24</v>
-      </c>
-      <c r="E99" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F99" s="32" t="s">
-        <v>245</v>
-      </c>
-      <c r="G99" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="H99" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="I99" s="32" t="s">
-        <v>246</v>
-      </c>
       <c r="J99" s="28" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K99" s="28" t="s">
         <v>17</v>
@@ -5006,34 +5006,34 @@
         <v>99</v>
       </c>
       <c r="B100" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="C100" t="s">
+        <v>295</v>
+      </c>
+      <c r="D100" t="s">
+        <v>24</v>
+      </c>
+      <c r="E100" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F100" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="G100" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="H100" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="C100" t="s">
-        <v>297</v>
-      </c>
-      <c r="D100" t="s">
-        <v>24</v>
-      </c>
-      <c r="E100" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F100" s="28" t="s">
+      <c r="I100" s="31" t="s">
         <v>248</v>
       </c>
-      <c r="G100" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="H100" s="28" t="s">
-        <v>249</v>
-      </c>
-      <c r="I100" s="31" t="s">
-        <v>250</v>
-      </c>
       <c r="J100" s="28" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K100" s="28" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="101" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5041,10 +5041,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="28" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C101" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D101" t="s">
         <v>24</v>
@@ -5074,31 +5074,31 @@
         <v>101</v>
       </c>
       <c r="B102" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="C102" t="s">
+        <v>252</v>
+      </c>
+      <c r="D102" t="s">
+        <v>24</v>
+      </c>
+      <c r="E102" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F102" s="31" t="s">
         <v>253</v>
       </c>
-      <c r="C102" t="s">
+      <c r="G102" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="H102" s="31" t="s">
         <v>254</v>
       </c>
-      <c r="D102" t="s">
-        <v>24</v>
-      </c>
-      <c r="E102" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F102" s="31" t="s">
+      <c r="I102" s="31" t="s">
         <v>255</v>
       </c>
-      <c r="G102" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="H102" s="31" t="s">
-        <v>256</v>
-      </c>
-      <c r="I102" s="31" t="s">
-        <v>257</v>
-      </c>
       <c r="J102" s="28" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K102" s="28" t="s">
         <v>42</v>
@@ -5109,10 +5109,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="28" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C103" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D103" t="s">
         <v>24</v>
@@ -5121,22 +5121,22 @@
         <v>13</v>
       </c>
       <c r="F103" s="34" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="I103" s="44" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="J103" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K103" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="104" spans="1:11" s="4" customFormat="1" ht="285" x14ac:dyDescent="0.25">
@@ -5144,34 +5144,34 @@
         <v>103</v>
       </c>
       <c r="B104" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="C104" t="s">
+        <v>297</v>
+      </c>
+      <c r="D104" t="s">
+        <v>24</v>
+      </c>
+      <c r="E104" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F104" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="G104" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="H104" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="C104" t="s">
-        <v>299</v>
-      </c>
-      <c r="D104" t="s">
-        <v>24</v>
-      </c>
-      <c r="E104" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F104" s="29" t="s">
+      <c r="I104" s="31" t="s">
         <v>261</v>
       </c>
-      <c r="G104" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="H104" s="29" t="s">
-        <v>262</v>
-      </c>
-      <c r="I104" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="J104" s="28" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K104" s="28" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="105" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -5179,34 +5179,34 @@
         <v>104</v>
       </c>
       <c r="B105" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="C105" t="s">
+        <v>263</v>
+      </c>
+      <c r="D105" t="s">
+        <v>24</v>
+      </c>
+      <c r="E105" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F105" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="C105" t="s">
+      <c r="G105" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="H105" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="D105" t="s">
-        <v>24</v>
-      </c>
-      <c r="E105" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F105" s="31" t="s">
+      <c r="I105" s="35" t="s">
         <v>266</v>
       </c>
-      <c r="G105" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="H105" s="31" t="s">
-        <v>267</v>
-      </c>
-      <c r="I105" s="35" t="s">
-        <v>268</v>
-      </c>
       <c r="J105" s="28" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K105" s="28" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="106" spans="1:11" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -5214,34 +5214,34 @@
         <v>105</v>
       </c>
       <c r="B106" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="C106" t="s">
+        <v>268</v>
+      </c>
+      <c r="D106" t="s">
+        <v>24</v>
+      </c>
+      <c r="E106" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F106" s="31" t="s">
         <v>269</v>
       </c>
-      <c r="C106" t="s">
+      <c r="G106" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="H106" s="31" t="s">
         <v>270</v>
       </c>
-      <c r="D106" t="s">
-        <v>24</v>
-      </c>
-      <c r="E106" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F106" s="31" t="s">
+      <c r="I106" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="G106" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="H106" s="31" t="s">
-        <v>272</v>
-      </c>
-      <c r="I106" s="31" t="s">
-        <v>273</v>
-      </c>
       <c r="J106" s="28" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K106" s="28" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="107" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5249,34 +5249,34 @@
         <v>106</v>
       </c>
       <c r="B107" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="C107" t="s">
+        <v>273</v>
+      </c>
+      <c r="D107" t="s">
+        <v>24</v>
+      </c>
+      <c r="E107" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F107" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="C107" t="s">
+      <c r="G107" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="H107" s="28" t="s">
         <v>275</v>
       </c>
-      <c r="D107" t="s">
-        <v>24</v>
-      </c>
-      <c r="E107" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F107" s="28" t="s">
+      <c r="I107" s="35" t="s">
         <v>276</v>
       </c>
-      <c r="G107" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="H107" s="28" t="s">
-        <v>277</v>
-      </c>
-      <c r="I107" s="35" t="s">
-        <v>278</v>
-      </c>
       <c r="J107" s="28" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K107" s="28" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="108" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5284,31 +5284,31 @@
         <v>107</v>
       </c>
       <c r="B108" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="C108" t="s">
+        <v>278</v>
+      </c>
+      <c r="D108" t="s">
+        <v>24</v>
+      </c>
+      <c r="E108" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F108" s="32" t="s">
         <v>279</v>
       </c>
-      <c r="C108" t="s">
+      <c r="G108" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H108" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I108" s="32" t="s">
         <v>280</v>
       </c>
-      <c r="D108" t="s">
-        <v>24</v>
-      </c>
-      <c r="E108" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F108" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="G108" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="H108" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="I108" s="32" t="s">
-        <v>282</v>
-      </c>
       <c r="J108" s="28" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K108" s="28" t="s">
         <v>17</v>
@@ -5319,10 +5319,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C109" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D109" t="s">
         <v>20</v>
@@ -5331,16 +5331,16 @@
         <v>13</v>
       </c>
       <c r="F109" s="42" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H109">
         <v>5</v>
       </c>
       <c r="I109" s="41" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J109" s="43" t="s">
         <v>16</v>
@@ -5429,8 +5429,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" topLeftCell="A51">
-      <selection activeCell="G56" sqref="G56"/>
+    <customSheetView guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" topLeftCell="A2">
+      <selection activeCell="G12" sqref="G12"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -5439,8 +5439,8 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{B7BE4B6F-CDC5-4AE8-A24C-80929B23A0EA}" topLeftCell="A2">
-      <selection activeCell="G12" sqref="G12"/>
+    <customSheetView guid="{9AC85045-6509-4A94-BC31-A1B440A0D150}" topLeftCell="A51">
+      <selection activeCell="G56" sqref="G56"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -5451,27 +5451,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5712,10 +5691,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9BE38D0-BD1C-4126-A2D1-5A24E80B0CB5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EF55999-2F9F-487E-85F2-88A3DAC30E62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5732,20 +5743,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EF55999-2F9F-487E-85F2-88A3DAC30E62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9BE38D0-BD1C-4126-A2D1-5A24E80B0CB5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>